<commit_message>
Design file continue. Satın almalar vs.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
@@ -61,6 +61,84 @@
       </text>
     </comment>
     <comment ref="H12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+This was selected high due to possible manufacturing problems.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+Depends on magnet selection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+Depends on magnet selection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="297">
   <si>
     <t>Power factor</t>
   </si>
@@ -2460,7 +2538,261 @@
     <t>Air gap length</t>
   </si>
   <si>
-    <t>Magnet and slot design</t>
+    <t>Magnet design</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>Tao se</t>
+  </si>
+  <si>
+    <t>bt ye bağlı</t>
+  </si>
+  <si>
+    <t>Peak back core flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cp</t>
+    </r>
+  </si>
+  <si>
+    <t>alfa s</t>
+  </si>
+  <si>
+    <t>B leri hesapla</t>
+  </si>
+  <si>
+    <t>Dos can be calculated later</t>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>rm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>rec</t>
+    </r>
+  </si>
+  <si>
+    <t>Magnet length</t>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>Air gap flux density (actual)</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>gap</t>
+    </r>
+  </si>
+  <si>
+    <t>Slot design</t>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2472,15 +2804,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2738,236 +3062,254 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3406,715 +3748,930 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="77" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="77" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="78" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" style="77" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" style="77" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="77" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="78" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" style="78" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" style="78" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" style="78" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="78" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.85546875" style="78" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="78" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" style="78" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="78"/>
+    <col min="1" max="1" width="21" style="70" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="69" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" style="70" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="70" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" style="70" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="64" t="s">
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="74" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-    </row>
-    <row r="2" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="66" t="s">
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="67">
+      <c r="C2" s="59">
         <v>8000</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="66" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="H2" s="67">
+      <c r="H2" s="59">
         <v>0.6</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="72">
+      <c r="M2" s="64">
         <v>3.1415926500000002</v>
       </c>
-      <c r="N2" s="67" t="s">
+      <c r="N2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="66" t="s">
+      <c r="O2" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="67" t="s">
+      <c r="P2" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="Q2" s="67">
+      <c r="Q2" s="59">
         <v>94</v>
       </c>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="59" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="59">
         <v>540</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="66" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="59">
         <v>35</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="67"/>
-      <c r="K3" s="66" t="s">
+      <c r="J3" s="59"/>
+      <c r="K3" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="67" t="s">
+      <c r="L3" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="M3" s="73">
+      <c r="M3" s="65">
         <v>1.7E-8</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="66" t="s">
+      <c r="O3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="67" t="s">
+      <c r="P3" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="67">
+      <c r="Q3" s="59">
         <v>0.9</v>
       </c>
-      <c r="R3" s="67" t="s">
+      <c r="R3" s="59" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="59">
         <v>4</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="66" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="59">
         <v>0.9</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="66" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="L4" s="67" t="s">
+      <c r="L4" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="M4" s="73">
+      <c r="M4" s="65">
         <v>1.2566289999999999E-6</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O4" s="66" t="s">
+      <c r="O4" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="Q4" s="67">
+      <c r="Q4" s="59">
         <v>98</v>
       </c>
-      <c r="R4" s="67" t="s">
+      <c r="R4" s="59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="59">
         <v>2</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="66" t="s">
+      <c r="E5" s="62"/>
+      <c r="F5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="59">
         <v>4</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="J5" s="67"/>
-      <c r="K5" s="66" t="s">
+      <c r="J5" s="59"/>
+      <c r="K5" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="73">
+      <c r="M5" s="65">
         <f>4*M2*0.0000001</f>
         <v>1.2566370599999999E-6</v>
       </c>
-      <c r="N5" s="67" t="s">
+      <c r="N5" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="67"/>
-    </row>
-    <row r="6" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="66" t="s">
+      <c r="O5" s="58"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="59"/>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="67">
+      <c r="C6" s="59">
         <v>3</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="66" t="s">
+      <c r="E6" s="62"/>
+      <c r="F6" s="58" t="s">
         <v>247</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="59">
         <v>1.8</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="I6" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-    </row>
-    <row r="7" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="66" t="s">
+      <c r="J6" s="59"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="59" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="59">
         <v>600</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-    </row>
-    <row r="8" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
+      <c r="E7" s="62"/>
+      <c r="F7" s="58" t="s">
+        <v>276</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="H7" s="59">
+        <v>1.8</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="59"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="59">
         <v>2</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="70"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-    </row>
-    <row r="9" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="E8" s="62"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="59">
         <v>2</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="70"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="67"/>
-    </row>
-    <row r="10" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-    </row>
-    <row r="11" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="E9" s="62"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="74" t="s">
         <v>257</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65" t="s">
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75" t="s">
         <v>272</v>
       </c>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-    </row>
-    <row r="12" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="66" t="s">
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="86" t="s">
+        <v>289</v>
+      </c>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="59" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="67">
+      <c r="C12" s="59">
         <f>C4*C8*C6</f>
         <v>24</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="74"/>
-      <c r="F12" s="68" t="s">
+      <c r="E12" s="66"/>
+      <c r="F12" s="60" t="s">
         <v>271</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="G12" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="H12" s="59">
         <v>1</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="84" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="67">
+      <c r="C13" s="59">
         <f>10*C8</f>
         <v>20</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="68" t="s">
+      <c r="E13" s="66"/>
+      <c r="F13" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="55" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" s="81">
+      <c r="G13" s="59" t="s">
+        <v>295</v>
+      </c>
+      <c r="H13" s="73">
         <f>M2*C20/C12</f>
         <v>26.271315346240922</v>
       </c>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="69"/>
-    </row>
-    <row r="14" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="66" t="s">
+      <c r="J13" s="85"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="59" t="s">
         <v>261</v>
       </c>
-      <c r="C14" s="67">
+      <c r="C14" s="59">
         <f>C12/(C13*C6)</f>
         <v>0.4</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-    </row>
-    <row r="15" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66" t="s">
+      <c r="E14" s="66"/>
+      <c r="F14" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>282</v>
+      </c>
+      <c r="H14" s="64">
+        <v>1</v>
+      </c>
+      <c r="I14" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="85"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="72">
+      <c r="C15" s="64">
         <f>H3*H4*2/M2</f>
         <v>20.053522852493302</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-    </row>
-    <row r="16" spans="1:18" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="66" t="s">
+      <c r="E15" s="66"/>
+      <c r="F15" s="82" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="H15" s="59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="85"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="72">
+      <c r="C16" s="64">
         <f>C2/(C7*2*M2/60)</f>
         <v>127.32395461900511</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-    </row>
-    <row r="17" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="66" t="s">
+      <c r="E16" s="66"/>
+      <c r="F16" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="H16" s="65">
+        <f>H15*M5</f>
+        <v>1.3823007660000001E-6</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" s="85"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="C17" s="75">
+      <c r="C17" s="67">
         <f>C16/(2*C15)*0.001</f>
         <v>3.174603174603175E-3</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="D17" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-    </row>
-    <row r="18" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="66" t="s">
+      <c r="E17" s="58"/>
+      <c r="F17" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="H17" s="59">
+        <v>3</v>
+      </c>
+      <c r="I17" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="58" t="s">
         <v>265</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="75">
+      <c r="C18" s="67">
         <f>C17*4/M2</f>
         <v>4.042030305365242E-3</v>
       </c>
-      <c r="D18" s="67" t="s">
+      <c r="D18" s="59" t="s">
         <v>267</v>
       </c>
-      <c r="E18" s="70"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-    </row>
-    <row r="19" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="66" t="s">
+      <c r="E18" s="62"/>
+      <c r="F18" s="87" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>290</v>
+      </c>
+      <c r="H18" s="59">
+        <v>0.7</v>
+      </c>
+      <c r="I18" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="80">
+      <c r="C19" s="72">
         <v>0.5</v>
       </c>
-      <c r="D19" s="67" t="s">
+      <c r="D19" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="76" t="s">
+      <c r="E19" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="68"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-    </row>
-    <row r="20" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="66" t="s">
+      <c r="F19" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="H19" s="64">
+        <f>2*Parameters!H8*Parameters!C16/'General Calculations'!C4</f>
+        <v>0.2199114855</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="J19" s="85"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="C20" s="80">
+      <c r="C20" s="72">
         <f>1000*(C18/C19)^(1/3)</f>
         <v>200.69806577558106</v>
       </c>
-      <c r="D20" s="67" t="s">
+      <c r="D20" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="70"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-    </row>
-    <row r="21" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="H20" s="64">
+        <f>H19*180/M2</f>
+        <v>12.6</v>
+      </c>
+      <c r="I20" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="J20" s="85"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="61" t="s">
         <v>268</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="73">
         <f>C20*C19</f>
         <v>100.34903288779053</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="D21" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-    </row>
-    <row r="22" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+      <c r="E21" s="61"/>
+      <c r="F21" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="G21" s="59" t="s">
+        <v>292</v>
+      </c>
+      <c r="H21" s="64">
+        <f>(H19*(C20/2-H12/2)+2*H12)*(C21+2*H12)/100</f>
+        <v>24.520729252821194</v>
+      </c>
+      <c r="I21" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="J21" s="85"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="61" t="s">
         <v>269</v>
       </c>
-      <c r="C22" s="81">
+      <c r="C22" s="73">
         <v>1.2</v>
       </c>
-      <c r="D22" s="79" t="s">
+      <c r="D22" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="F22" s="68"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-    </row>
-    <row r="23" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="68" t="s">
+      <c r="F22" s="82" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>294</v>
+      </c>
+      <c r="H22" s="64">
+        <f>(H19*(C20/2-H12/2)+2*H12)*(C21+2*H12)/100</f>
+        <v>24.520729252821194</v>
+      </c>
+      <c r="I22" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="J22" s="61"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="C23" s="81">
+      <c r="C23" s="73">
         <f>C20*C22</f>
         <v>240.83767893069725</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="69"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-    </row>
-    <row r="24" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="68"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-    </row>
-    <row r="25" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="82" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="H23" s="64">
+        <f>H22/H21</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="71"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="60"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="82" t="s">
+        <v>205</v>
+      </c>
+      <c r="G24" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="64">
+        <f>H22*H12/(H21*H17)</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="I24" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="61"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="60" t="s">
+        <v>287</v>
+      </c>
+      <c r="G25" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="H25" s="61">
+        <f>M28*M32*H31/(1+H32*M30*M29)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="70" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K29" s="70" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K30" s="70" t="s">
+        <v>274</v>
+      </c>
+      <c r="L30" s="70" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K31" s="70" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K33" s="70" t="s">
+        <v>279</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="F11:J11"/>
+    <mergeCell ref="K11:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4128,7 +4685,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4316,12 +4873,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -4582,35 +5139,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62" t="s">
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="59" t="s">
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="77" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="61"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="79"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4832,7 +5389,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="81" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -4899,7 +5456,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="63"/>
+      <c r="J6" s="81"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -5126,20 +5683,20 @@
       <c r="E10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62" t="s">
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -5204,7 +5761,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="63" t="s">
+      <c r="O11" s="81" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -5271,7 +5828,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="63"/>
+      <c r="O12" s="81"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -5337,7 +5894,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="63"/>
+      <c r="O13" s="81"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -5502,13 +6059,13 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
       <c r="K17" s="29" t="s">
         <v>140</v>
       </c>
@@ -5747,13 +6304,13 @@
         <v>15</v>
       </c>
       <c r="J23" s="46"/>
-      <c r="K23" s="62" t="s">
+      <c r="K23" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="44"/>

</xml_diff>

<commit_message>
Mass, volume, power density, resistance etc added to the design file. Induced voltage harmonic spectrum analysis for maxwell output.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R12" authorId="0" shapeId="0">
+    <comment ref="R13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="383">
   <si>
     <t>Power factor</t>
   </si>
@@ -3329,6 +3329,171 @@
     </r>
   </si>
   <si>
+    <t>Ω</t>
+  </si>
+  <si>
+    <t>Peak flux density (fund)</t>
+  </si>
+  <si>
+    <t>Average flux density (fund)</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>p-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>avg-1</t>
+    </r>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Applied volt</t>
+  </si>
+  <si>
+    <t>Volume &amp; Mass</t>
+  </si>
+  <si>
+    <t>Magnet volume</t>
+  </si>
+  <si>
+    <t>Iron volume</t>
+  </si>
+  <si>
+    <t>Copper volume</t>
+  </si>
+  <si>
+    <t>Bore volume</t>
+  </si>
+  <si>
+    <t>Machine volume</t>
+  </si>
+  <si>
+    <r>
+      <t>cm</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>is</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>os</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase resistance (module)</t>
+  </si>
+  <si>
     <r>
       <t>R</t>
     </r>
@@ -3341,37 +3506,37 @@
         <family val="1"/>
         <charset val="162"/>
       </rPr>
-      <t>ph</t>
-    </r>
-  </si>
-  <si>
-    <t>Ω</t>
-  </si>
-  <si>
-    <t>Peak flux density (fund)</t>
-  </si>
-  <si>
-    <t>Average flux density (fund)</t>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>Copper density</t>
+  </si>
+  <si>
+    <t>Core density</t>
+  </si>
+  <si>
+    <t>Magnet density</t>
+  </si>
+  <si>
+    <r>
+      <t>g/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Garamond"/>
         <family val="1"/>
         <charset val="162"/>
       </rPr>
-      <t>p-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
     </r>
     <r>
       <rPr>
@@ -3382,20 +3547,103 @@
         <family val="1"/>
         <charset val="162"/>
       </rPr>
-      <t>avg-1</t>
-    </r>
-  </si>
-  <si>
-    <t>Total flux per pole (total)</t>
-  </si>
-  <si>
-    <t>Total flux per pole (fund)</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Applied volt</t>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <t>Magnet mass</t>
+  </si>
+  <si>
+    <t>Iron mass</t>
+  </si>
+  <si>
+    <t>Copper mass</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
 </sst>
 </file>
@@ -3409,9 +3657,9 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.00000000"/>
     <numFmt numFmtId="169" formatCode="0.0000000000"/>
-    <numFmt numFmtId="175" formatCode="#,##0.000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3547,8 +3795,26 @@
       <family val="1"/>
       <charset val="162"/>
     </font>
+    <font>
+      <strike/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3612,6 +3878,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3714,10 +3986,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3880,9 +4153,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4010,67 +4280,10 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="14" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4086,8 +4299,77 @@
     <xf numFmtId="2" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4567,1508 +4849,1592 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="71" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="70" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" style="70" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="70" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" style="70" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" style="71" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="71" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" style="71" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="71" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="71" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="71" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="71"/>
+    <col min="1" max="1" width="22.5703125" style="70" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="69" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" style="70" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="70" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="113" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="106" t="s">
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="113" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="106" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="113" t="s">
         <v>333</v>
       </c>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="59">
         <v>8000</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="59" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="59">
         <v>0.6</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="60"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="65">
+      <c r="M2" s="64">
         <v>3.1415926500000002</v>
       </c>
-      <c r="N2" s="60" t="s">
+      <c r="N2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="59" t="s">
+      <c r="O2" s="59"/>
+      <c r="P2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="60" t="s">
+      <c r="Q2" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="R2" s="60">
+      <c r="R2" s="59">
         <f>C4*C8*C6</f>
         <v>24</v>
       </c>
-      <c r="S2" s="60" t="s">
+      <c r="S2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="67"/>
+      <c r="T2" s="66"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="60">
+      <c r="C3" s="59">
         <v>540</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="59" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="H3" s="60">
+      <c r="H3" s="59">
         <v>35</v>
       </c>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="59" t="s">
+      <c r="J3" s="59"/>
+      <c r="K3" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="M3" s="66">
+      <c r="M3" s="65">
         <v>1.7E-8</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="60"/>
-      <c r="P3" s="59" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="60" t="s">
+      <c r="Q3" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="60">
+      <c r="R3" s="59">
         <f>10*C8</f>
         <v>20</v>
       </c>
-      <c r="S3" s="60" t="s">
+      <c r="S3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="67"/>
+      <c r="T3" s="66"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="60">
+      <c r="C4" s="59">
         <v>4</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="60">
+      <c r="H4" s="59">
         <v>0.9</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="60"/>
-      <c r="K4" s="59" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="M4" s="66">
+      <c r="M4" s="65">
         <v>1.2566289999999999E-6</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="59" t="s">
+      <c r="O4" s="59"/>
+      <c r="P4" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="R4" s="65">
+      <c r="R4" s="64">
         <f>H3*H4*2/M2</f>
         <v>20.053522852493302</v>
       </c>
-      <c r="S4" s="60" t="s">
+      <c r="S4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="T4" s="67"/>
+      <c r="T4" s="66"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="59">
         <v>2</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="59" t="s">
+      <c r="E5" s="62"/>
+      <c r="F5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="59">
         <v>4</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="J5" s="60"/>
-      <c r="K5" s="59" t="s">
+      <c r="J5" s="59"/>
+      <c r="K5" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="L5" s="60" t="s">
+      <c r="L5" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="66">
+      <c r="M5" s="65">
         <f>4*M2*0.0000001</f>
         <v>1.2566370599999999E-6</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="60"/>
-      <c r="P5" s="59" t="s">
+      <c r="O5" s="59"/>
+      <c r="P5" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="Q5" s="60" t="s">
+      <c r="Q5" s="59" t="s">
         <v>260</v>
       </c>
-      <c r="R5" s="65">
+      <c r="R5" s="64">
         <f>C2/(C7*2*M2/60)</f>
         <v>127.32395461900511</v>
       </c>
-      <c r="S5" s="60" t="s">
+      <c r="S5" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="67"/>
-    </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
+      <c r="T5" s="66"/>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="59">
         <v>3</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="59" t="s">
+      <c r="E6" s="62"/>
+      <c r="F6" s="58" t="s">
         <v>247</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="59">
         <v>1.8</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="112" t="s">
-        <v>246</v>
-      </c>
-      <c r="L6" s="113"/>
-      <c r="M6" s="113"/>
-      <c r="N6" s="113"/>
-      <c r="O6" s="114"/>
-      <c r="P6" s="59" t="s">
+      <c r="J6" s="59"/>
+      <c r="K6" s="60" t="s">
+        <v>368</v>
+      </c>
+      <c r="L6" s="61" t="s">
+        <v>372</v>
+      </c>
+      <c r="M6" s="61">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>371</v>
+      </c>
+      <c r="O6" s="60"/>
+      <c r="P6" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="Q6" s="60" t="s">
+      <c r="Q6" s="59" t="s">
         <v>261</v>
       </c>
-      <c r="R6" s="68">
+      <c r="R6" s="67">
         <f>R5/(2*R4)*0.001</f>
         <v>3.174603174603175E-3</v>
       </c>
-      <c r="S6" s="60" t="s">
+      <c r="S6" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="T6" s="59"/>
-    </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="T6" s="58"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="59" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="59">
         <v>600</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="59" t="s">
+      <c r="E7" s="62"/>
+      <c r="F7" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="59" t="s">
         <v>271</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="59">
         <v>1.3</v>
       </c>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="60"/>
-      <c r="K7" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="60" t="s">
-        <v>250</v>
-      </c>
-      <c r="M7" s="60">
-        <v>94</v>
-      </c>
-      <c r="N7" s="60" t="s">
-        <v>51</v>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="L7" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61" t="s">
+        <v>371</v>
       </c>
       <c r="O7" s="60"/>
-      <c r="P7" s="59" t="s">
+      <c r="P7" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="Q7" s="60" t="s">
+      <c r="Q7" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="R7" s="68">
+      <c r="R7" s="67">
         <f>R6*4/M2</f>
         <v>4.042030305365242E-3</v>
       </c>
-      <c r="S7" s="60" t="s">
+      <c r="S7" s="59" t="s">
         <v>265</v>
       </c>
-      <c r="T7" s="63"/>
-    </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="T7" s="62"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="60">
+      <c r="C8" s="59">
         <v>2</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="60">
-        <v>0.9</v>
-      </c>
-      <c r="N8" s="60" t="s">
+      <c r="E8" s="62"/>
+      <c r="F8" s="119" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="L8" s="61" t="s">
+        <v>373</v>
+      </c>
+      <c r="M8" s="61">
+        <v>7.4</v>
+      </c>
+      <c r="N8" s="61" t="s">
+        <v>371</v>
+      </c>
+      <c r="O8" s="60"/>
+      <c r="P8" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="S8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="R8" s="73">
-        <v>0.5</v>
-      </c>
-      <c r="S8" s="60" t="s">
+      <c r="T8" s="68" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="59">
+        <v>2</v>
+      </c>
+      <c r="D9" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="T8" s="69" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="60">
-        <v>2</v>
-      </c>
-      <c r="D9" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="60" t="s">
-        <v>254</v>
-      </c>
-      <c r="M9" s="60">
-        <v>98</v>
-      </c>
-      <c r="N9" s="60" t="s">
+      <c r="E9" s="62"/>
+      <c r="F9" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="H9" s="59">
+        <v>94</v>
+      </c>
+      <c r="I9" s="59" t="s">
         <v>51</v>
       </c>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
       <c r="O9" s="60"/>
-      <c r="P9" s="59" t="s">
+      <c r="P9" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="60" t="s">
+      <c r="Q9" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="R9" s="73">
+      <c r="R9" s="72">
         <f>1000*(R7/R8)^(1/3)</f>
         <v>200.69806577558106</v>
       </c>
-      <c r="S9" s="60" t="s">
+      <c r="S9" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="T9" s="63"/>
+      <c r="T9" s="62"/>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="59">
+        <v>0.9</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
       <c r="O10" s="60"/>
-      <c r="P10" s="59" t="s">
+      <c r="P10" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="Q10" s="62" t="s">
+      <c r="Q10" s="61" t="s">
         <v>266</v>
       </c>
-      <c r="R10" s="74">
+      <c r="R10" s="73">
         <f>R9*R8</f>
         <v>100.34903288779053</v>
       </c>
-      <c r="S10" s="62" t="s">
+      <c r="S10" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T10" s="62"/>
-      <c r="U10" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="V10" s="71">
-        <f>M17*SQRT(3)*4</f>
+      <c r="T10" s="61"/>
+      <c r="U10" s="70" t="s">
+        <v>353</v>
+      </c>
+      <c r="V10" s="70">
+        <f>M18*SQRT(3)*4</f>
         <v>688.74706159105506</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="H11" s="59">
+        <v>98</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="59"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="114" t="s">
         <v>269</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107" t="s">
+      <c r="B12" s="114"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="119" t="s">
         <v>280</v>
       </c>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="108" t="s">
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="115" t="s">
         <v>317</v>
       </c>
-      <c r="L11" s="109"/>
-      <c r="M11" s="109"/>
-      <c r="N11" s="109"/>
-      <c r="O11" s="110"/>
-      <c r="P11" s="107" t="s">
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="117"/>
+      <c r="P12" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="Q11" s="107"/>
-      <c r="R11" s="107"/>
-      <c r="S11" s="107"/>
-      <c r="T11" s="107"/>
-    </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61" t="s">
+      <c r="Q12" s="114"/>
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="60" t="s">
         <v>268</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B13" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="C12" s="60">
+      <c r="C13" s="59">
         <v>1</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D13" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E13" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="F12" s="61" t="s">
+      <c r="F13" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G13" s="59" t="s">
         <v>286</v>
       </c>
-      <c r="H12" s="74">
+      <c r="H13" s="73">
         <f>M2*R9/R2</f>
         <v>26.271315346240922</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I13" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="75" t="s">
+      <c r="J13" s="61"/>
+      <c r="K13" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="L12" s="60" t="s">
+      <c r="L13" s="59" t="s">
         <v>296</v>
       </c>
-      <c r="M12" s="60">
+      <c r="M13" s="59">
         <v>0.93300000000000005</v>
       </c>
-      <c r="N12" s="60" t="s">
+      <c r="N13" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="69" t="s">
+      <c r="O13" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="P12" s="75" t="s">
+      <c r="P13" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="Q12" s="60" t="s">
+      <c r="Q13" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="R12" s="65">
-        <f>1000*SQRT(2/(2*M2*M14*M4/M3))</f>
+      <c r="R13" s="64">
+        <f>1000*SQRT(2/(2*M2*M15*M4/M3))</f>
         <v>6.562147464226471</v>
       </c>
-      <c r="S12" s="60" t="s">
+      <c r="S13" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="T12" s="62"/>
-    </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
+      <c r="T13" s="61"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B14" s="59" t="s">
         <v>273</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C14" s="64">
         <v>1.25</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D14" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="61" t="s">
+      <c r="E14" s="61"/>
+      <c r="F14" s="60" t="s">
         <v>295</v>
       </c>
-      <c r="G13" s="60" t="s">
+      <c r="G14" s="59" t="s">
         <v>323</v>
       </c>
-      <c r="H13" s="82">
-        <f>C24/H6</f>
+      <c r="H14" s="81">
+        <f>C25/H6</f>
         <v>0.50170274872293841</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I14" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="61"/>
-      <c r="K13" s="75" t="s">
+      <c r="J14" s="60"/>
+      <c r="K14" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="60" t="s">
+      <c r="L14" s="59" t="s">
         <v>307</v>
       </c>
-      <c r="M13" s="84">
-        <f>0.001*2*R9*R10*C25/R3</f>
+      <c r="M14" s="83">
+        <f>0.001*2*R9*R10*C26/R3</f>
         <v>1.9998309272554273</v>
       </c>
-      <c r="N13" s="60" t="s">
+      <c r="N14" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="63"/>
-      <c r="P13" s="61" t="s">
+      <c r="O14" s="62"/>
+      <c r="P14" s="60" t="s">
         <v>337</v>
       </c>
-      <c r="Q13" s="62" t="s">
+      <c r="Q14" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="R13" s="102">
-        <f>2*SQRT(M19/(M2*H5))</f>
+      <c r="R14" s="101">
+        <f>2*SQRT(M20/(M2*H5))</f>
         <v>1.4425038006176998</v>
       </c>
-      <c r="S13" s="62" t="s">
+      <c r="S14" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T13" s="62"/>
-    </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="75" t="s">
+      <c r="T14" s="61"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B15" s="59" t="s">
         <v>274</v>
       </c>
-      <c r="C14" s="60">
+      <c r="C15" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D15" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="85" t="s">
+      <c r="E15" s="61"/>
+      <c r="F15" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G15" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="H14" s="86">
-        <f>H13*H12</f>
+      <c r="H15" s="85">
+        <f>H14*H13</f>
         <v>13.180391121776184</v>
       </c>
-      <c r="I14" s="87" t="s">
+      <c r="I15" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="87"/>
-      <c r="K14" s="71" t="s">
+      <c r="J15" s="86"/>
+      <c r="K15" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="60" t="s">
+      <c r="L15" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="M14" s="60">
+      <c r="M15" s="59">
         <f>R3*C7/120</f>
         <v>100</v>
       </c>
-      <c r="N14" s="60" t="s">
+      <c r="N15" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61" t="s">
+      <c r="O15" s="60"/>
+      <c r="P15" s="60" t="s">
         <v>335</v>
       </c>
-      <c r="Q14" s="62" t="s">
+      <c r="Q15" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="R14" s="62">
+      <c r="R15" s="61">
         <v>14</v>
       </c>
-      <c r="S14" s="62" t="s">
+      <c r="S15" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="T14" s="123" t="s">
+      <c r="T15" s="122" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="75" t="s">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B16" s="59" t="s">
         <v>275</v>
       </c>
-      <c r="C15" s="66">
-        <f>C14*M5</f>
+      <c r="C16" s="65">
+        <f>C15*M5</f>
         <v>1.3823007660000001E-6</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="62"/>
-      <c r="F15" s="88" t="s">
+      <c r="E16" s="61"/>
+      <c r="F16" s="87" t="s">
         <v>140</v>
       </c>
-      <c r="G15" s="89" t="s">
+      <c r="G16" s="88" t="s">
         <v>299</v>
       </c>
-      <c r="H15" s="90">
-        <f>H12-H14</f>
+      <c r="H16" s="89">
+        <f>H13-H15</f>
         <v>13.090924224464738</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I16" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="83"/>
-      <c r="K15" s="59" t="s">
+      <c r="J16" s="82"/>
+      <c r="K16" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="L15" s="94" t="s">
+      <c r="L16" s="93" t="s">
         <v>298</v>
       </c>
-      <c r="M15" s="94">
+      <c r="M16" s="93">
         <v>60</v>
       </c>
-      <c r="N15" s="94" t="s">
+      <c r="N16" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="94" t="s">
+      <c r="O16" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="P15" s="61" t="s">
+      <c r="P16" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="Q15" s="62" t="s">
+      <c r="Q16" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="R15" s="122">
+      <c r="R16" s="106">
         <v>1.6281399999999999</v>
       </c>
-      <c r="S15" s="62" t="s">
+      <c r="S16" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T15" s="125"/>
-      <c r="U15" s="71" t="s">
+      <c r="T16" s="123"/>
+      <c r="U16" s="70" t="s">
         <v>288</v>
       </c>
-      <c r="V15" s="71">
+      <c r="V16" s="70">
         <v>0.99</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="60" t="s">
         <v>276</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B17" s="59" t="s">
         <v>277</v>
       </c>
-      <c r="C16" s="60">
+      <c r="C17" s="59">
         <v>3</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D17" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E17" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="F16" s="75" t="s">
+      <c r="F17" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="G16" s="60" t="s">
+      <c r="G17" s="59" t="s">
         <v>301</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H17" s="59">
         <v>4</v>
       </c>
-      <c r="I16" s="60" t="s">
+      <c r="I17" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J16" s="111" t="s">
+      <c r="J17" s="118" t="s">
         <v>178</v>
       </c>
-      <c r="K16" s="59" t="s">
+      <c r="K17" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="60" t="s">
+      <c r="L17" s="59" t="s">
         <v>300</v>
       </c>
-      <c r="M16" s="60">
-        <f>M15*C8*C9/2</f>
+      <c r="M17" s="59">
+        <f>M16*C8*C9/2</f>
         <v>120</v>
       </c>
-      <c r="N16" s="60" t="s">
+      <c r="N17" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="63"/>
-      <c r="P16" s="61" t="s">
+      <c r="O17" s="62"/>
+      <c r="P17" s="60" t="s">
         <v>340</v>
       </c>
-      <c r="Q16" s="60" t="s">
+      <c r="Q17" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="R16" s="62">
+      <c r="R17" s="61">
         <v>8.282</v>
       </c>
-      <c r="S16" s="60" t="s">
+      <c r="S17" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="T16" s="124"/>
-      <c r="U16" s="71" t="s">
+      <c r="T17" s="124"/>
+      <c r="U17" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="V16" s="71">
+      <c r="V17" s="70">
         <v>1.01</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="76" t="s">
+    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B18" s="59" t="s">
         <v>281</v>
       </c>
-      <c r="C17" s="60">
+      <c r="C18" s="59">
         <v>0.7</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E18" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="75" t="s">
+      <c r="F18" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="G17" s="60" t="s">
+      <c r="G18" s="59" t="s">
         <v>303</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H18" s="59">
         <v>1.5</v>
       </c>
-      <c r="I17" s="60" t="s">
+      <c r="I18" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="111"/>
-      <c r="K17" s="95" t="s">
+      <c r="J18" s="118"/>
+      <c r="K18" s="94" t="s">
         <v>143</v>
       </c>
-      <c r="L17" s="96" t="s">
+      <c r="L18" s="95" t="s">
         <v>302</v>
       </c>
-      <c r="M17" s="97">
-        <f>4.44*M16*M14*M13*M12/1000</f>
+      <c r="M18" s="96">
+        <f>4.44*M17*M15*M14*M13/1000</f>
         <v>99.41207535328985</v>
       </c>
-      <c r="N17" s="96" t="s">
+      <c r="N18" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="98"/>
-      <c r="P17" s="61" t="s">
+      <c r="O18" s="97"/>
+      <c r="P18" s="60" t="s">
         <v>342</v>
       </c>
-      <c r="Q17" s="62" t="s">
+      <c r="Q18" s="61" t="s">
         <v>344</v>
       </c>
-      <c r="R17" s="82">
-        <f>2*R10*V17+2*H12</f>
-        <v>263.27559975684193</v>
-      </c>
-      <c r="S17" s="62" t="s">
+      <c r="R18" s="81">
+        <f>2*R10*V18+2*H13</f>
+        <v>273.31050304562103</v>
+      </c>
+      <c r="S18" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T17" s="62"/>
-      <c r="U17" s="71" t="s">
+      <c r="T18" s="61"/>
+      <c r="U18" s="70" t="s">
         <v>345</v>
       </c>
-      <c r="V17" s="71">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+      <c r="V18" s="70">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B19" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="C18" s="65">
-        <f>2*M2*C17/R3</f>
+      <c r="C19" s="64">
+        <f>2*M2*C18/R3</f>
         <v>0.2199114855</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="75" t="s">
+      <c r="E19" s="61"/>
+      <c r="F19" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="60" t="s">
+      <c r="G19" s="59" t="s">
         <v>305</v>
       </c>
-      <c r="H18" s="60">
+      <c r="H19" s="59">
         <v>1.5</v>
       </c>
-      <c r="I18" s="60" t="s">
+      <c r="I19" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="111"/>
-      <c r="K18" s="59" t="s">
+      <c r="J19" s="118"/>
+      <c r="K19" s="58" t="s">
         <v>334</v>
       </c>
-      <c r="L18" s="60" t="s">
+      <c r="L19" s="59" t="s">
         <v>304</v>
       </c>
-      <c r="M18" s="65">
-        <f>M17*C4*SQRT(3)*SQRT(2)</f>
+      <c r="M19" s="64">
+        <f>M18*C4*SQRT(3)*SQRT(2)</f>
         <v>974.03543554668749</v>
       </c>
-      <c r="N18" s="60" t="s">
+      <c r="N19" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61" t="s">
+      <c r="O19" s="60"/>
+      <c r="P19" s="60" t="s">
         <v>343</v>
       </c>
-      <c r="Q18" s="62" t="s">
+      <c r="Q19" s="61" t="s">
         <v>346</v>
       </c>
-      <c r="R18" s="82">
-        <f>R17*M16/1000</f>
-        <v>31.593071970821033</v>
-      </c>
-      <c r="S18" s="62" t="s">
+      <c r="R19" s="81">
+        <f>R18*M17/1000</f>
+        <v>32.797260365474528</v>
+      </c>
+      <c r="S19" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="T18" s="62"/>
-    </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="75" t="s">
+      <c r="T19" s="61"/>
+    </row>
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B20" s="59" t="s">
         <v>282</v>
       </c>
-      <c r="C19" s="65">
-        <f>C18*180/M2</f>
+      <c r="C20" s="64">
+        <f>C19*180/M2</f>
         <v>12.6</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D20" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="75" t="s">
+      <c r="E20" s="61"/>
+      <c r="F20" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G20" s="59" t="s">
         <v>306</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H20" s="59">
         <v>1.5</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I20" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="111"/>
-      <c r="K19" s="98" t="s">
+      <c r="J20" s="118"/>
+      <c r="K20" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="L19" s="96" t="s">
+      <c r="L20" s="95" t="s">
         <v>316</v>
       </c>
-      <c r="M19" s="99">
-        <f>H5*H25/(2*M15)</f>
+      <c r="M20" s="98">
+        <f>H5*H26/(2*M16)</f>
         <v>6.5370800679981835</v>
       </c>
-      <c r="N19" s="100" t="s">
+      <c r="N20" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="100"/>
-      <c r="P19" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q19" s="62" t="s">
+      <c r="O20" s="99"/>
+      <c r="P20" s="60" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q20" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="R20" s="81">
+        <f>R17*R19/1000</f>
+        <v>0.27162691034686004</v>
+      </c>
+      <c r="S20" s="59" t="s">
         <v>347</v>
       </c>
-      <c r="R19" s="82">
-        <f>R16*R18/1000</f>
-        <v>0.26165382206233978</v>
-      </c>
-      <c r="S19" s="60" t="s">
+      <c r="T20" s="61"/>
+      <c r="U20" s="70" t="s">
+        <v>292</v>
+      </c>
+      <c r="V20" s="70" t="s">
+        <v>293</v>
+      </c>
+      <c r="W20" s="135" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" s="64">
+        <f>(C19*(R9/2-C13/2)+2*C13)*(R10+2*C13)/100</f>
+        <v>24.520729252821194</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" s="61"/>
+      <c r="F21" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="93" t="s">
+        <v>311</v>
+      </c>
+      <c r="H21" s="93">
+        <v>20</v>
+      </c>
+      <c r="I21" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="100"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="61"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="61"/>
+      <c r="U21" s="70" t="s">
+        <v>294</v>
+      </c>
+      <c r="V21" s="70" t="s">
+        <v>289</v>
+      </c>
+      <c r="W21" s="135" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="59" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="64">
+        <f>(C19*(R9/2-C13/2)+2*C13)*(R10+2*C13)/100</f>
+        <v>24.520729252821194</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="E22" s="61"/>
+      <c r="F22" s="60" t="s">
+        <v>308</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>309</v>
+      </c>
+      <c r="H22" s="81">
+        <f>R9+(H18+H19+H20+H21)*2</f>
+        <v>249.69806577558106</v>
+      </c>
+      <c r="I22" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="60"/>
+      <c r="K22" s="114" t="s">
+        <v>319</v>
+      </c>
+      <c r="L22" s="114"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="114"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="115" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q22" s="116"/>
+      <c r="R22" s="116"/>
+      <c r="S22" s="116"/>
+      <c r="T22" s="117"/>
+      <c r="W22" s="70" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="64">
+        <f>C22/C21</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="71"/>
+      <c r="F23" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>324</v>
+      </c>
+      <c r="H23" s="64">
+        <f>M2*H22/R2</f>
+        <v>32.68540033999092</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" s="60"/>
+      <c r="K23" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="108" t="s">
+        <v>352</v>
+      </c>
+      <c r="M23" s="109">
+        <f>C26</f>
+        <v>0.99297177075985155</v>
+      </c>
+      <c r="N23" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="108"/>
+      <c r="P23" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q23" s="61" t="s">
+        <v>361</v>
+      </c>
+      <c r="R23" s="81">
+        <f>C17*R10*C18*M2*(R9-C13)/R3/1000</f>
+        <v>6.6103768836310586</v>
+      </c>
+      <c r="S23" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="T23" s="61"/>
+    </row>
+    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="64">
+        <f>C22*C13/(C21*C17)</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="61"/>
+      <c r="F24" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="59" t="s">
+        <v>312</v>
+      </c>
+      <c r="H24" s="64">
+        <f>H23-H15</f>
+        <v>19.505009218214738</v>
+      </c>
+      <c r="I24" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" s="62"/>
+      <c r="K24" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="110" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="111">
+        <f>R2*M16*C9*M20/(M2*R9)</f>
+        <v>29.859548249533173</v>
+      </c>
+      <c r="N24" s="110" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="110"/>
+      <c r="P24" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q24" s="61" t="s">
+        <v>362</v>
+      </c>
+      <c r="R24" s="81"/>
+      <c r="S24" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="T24" s="61"/>
+    </row>
+    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="C25" s="101">
+        <f>V16*C14*C23/(1+V17*C15*C24)</f>
+        <v>0.9030649477012892</v>
+      </c>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="H25" s="64">
+        <f>(H24+H15)*H21/2</f>
+        <v>326.85400339990917</v>
+      </c>
+      <c r="I25" s="59" t="s">
+        <v>314</v>
+      </c>
+      <c r="J25" s="59"/>
+      <c r="K25" s="92" t="s">
+        <v>320</v>
+      </c>
+      <c r="L25" s="108"/>
+      <c r="M25" s="108"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q25" s="61" t="s">
+        <v>363</v>
+      </c>
+      <c r="R25" s="81">
+        <f>R19*C6*C4*(R16/2)^2*M2</f>
+        <v>819.39288162356786</v>
+      </c>
+      <c r="S25" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="T25" s="61"/>
+    </row>
+    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="C26" s="101">
+        <f>C25*C18*M2/2</f>
+        <v>0.99297177075985155</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="60" t="s">
+        <v>310</v>
+      </c>
+      <c r="G26" s="59" t="s">
+        <v>315</v>
+      </c>
+      <c r="H26" s="81">
+        <f>H25*H2</f>
+        <v>196.11240203994549</v>
+      </c>
+      <c r="I26" s="59" t="s">
+        <v>314</v>
+      </c>
+      <c r="J26" s="60"/>
+      <c r="K26" s="90" t="s">
+        <v>321</v>
+      </c>
+      <c r="L26" s="91"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="91"/>
+      <c r="O26" s="91"/>
+      <c r="P26" s="60" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q26" s="61" t="s">
+        <v>364</v>
+      </c>
+      <c r="R26" s="81">
+        <f>M2*R9*R10/1000</f>
+        <v>63.271226104450712</v>
+      </c>
+      <c r="S26" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="T26" s="61"/>
+    </row>
+    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="131" t="s">
         <v>348</v>
       </c>
-      <c r="T19" s="62"/>
-      <c r="U19" s="71" t="s">
-        <v>292</v>
-      </c>
-      <c r="V19" s="71" t="s">
-        <v>293</v>
-      </c>
-      <c r="W19" s="71" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="B20" s="60" t="s">
-        <v>283</v>
-      </c>
-      <c r="C20" s="65">
-        <f>(C18*(R9/2-C12/2)+2*C12)*(R10+2*C12)/100</f>
-        <v>24.520729252821194</v>
-      </c>
-      <c r="D20" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="94" t="s">
-        <v>311</v>
-      </c>
-      <c r="H20" s="94">
-        <v>20</v>
-      </c>
-      <c r="I20" s="94" t="s">
+      <c r="B27" s="132" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="133">
+        <f>4*C25/M2*(COS(M2*C18/2))</f>
+        <v>0.52200645161955517</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="115" t="s">
+        <v>318</v>
+      </c>
+      <c r="G27" s="116"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="L27" s="104"/>
+      <c r="M27" s="105">
+        <f>M20*M18</f>
+        <v>649.86469631032458</v>
+      </c>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="60" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q27" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="R27" s="81">
+        <f>M2*H29*R10/1000</f>
+        <v>84.472105812205513</v>
+      </c>
+      <c r="S27" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="T27" s="61"/>
+    </row>
+    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="131" t="s">
+        <v>349</v>
+      </c>
+      <c r="B28" s="132" t="s">
+        <v>351</v>
+      </c>
+      <c r="C28" s="134">
+        <f>C27*2/M2</f>
+        <v>0.33231962878418064</v>
+      </c>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H28" s="23">
+        <f>(H6/H7)*H15/2</f>
+        <v>9.1248861612296661</v>
+      </c>
+      <c r="I28" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="94" t="s">
-        <v>178</v>
-      </c>
-      <c r="K20" s="101"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="101"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="101"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="71" t="s">
-        <v>294</v>
-      </c>
-      <c r="V20" s="71" t="s">
-        <v>289</v>
-      </c>
-      <c r="W20" s="71" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>285</v>
-      </c>
-      <c r="C21" s="65">
-        <f>(C18*(R9/2-C12/2)+2*C12)*(R10+2*C12)/100</f>
-        <v>24.520729252821194</v>
-      </c>
-      <c r="D21" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="61" t="s">
-        <v>308</v>
-      </c>
-      <c r="G21" s="60" t="s">
-        <v>309</v>
-      </c>
-      <c r="H21" s="82">
-        <f>R9+(H17+H18+H19+H20)*2</f>
-        <v>249.69806577558106</v>
-      </c>
-      <c r="I21" s="62" t="s">
+      <c r="J28" s="60"/>
+      <c r="K28" s="103" t="s">
+        <v>327</v>
+      </c>
+      <c r="L28" s="104"/>
+      <c r="M28" s="105">
+        <f>M27*C4*C6</f>
+        <v>7798.3763557238944</v>
+      </c>
+      <c r="N28" s="104"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q28" s="61" t="s">
+        <v>378</v>
+      </c>
+      <c r="R28" s="81">
+        <f>R23*M8</f>
+        <v>48.916788938869836</v>
+      </c>
+      <c r="S28" s="61" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="60"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="H29" s="73">
+        <f>H22+H28*2</f>
+        <v>267.94783809804039</v>
+      </c>
+      <c r="I29" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="J21" s="61"/>
-      <c r="K21" s="108" t="s">
-        <v>318</v>
-      </c>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
-      <c r="O21" s="110"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
-      <c r="T21" s="62"/>
-      <c r="W21" s="71" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="75" t="s">
-        <v>203</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>287</v>
-      </c>
-      <c r="C22" s="65">
-        <f>C21/C20</f>
-        <v>1</v>
-      </c>
-      <c r="D22" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="72"/>
-      <c r="F22" s="76" t="s">
-        <v>149</v>
-      </c>
-      <c r="G22" s="60" t="s">
-        <v>324</v>
-      </c>
-      <c r="H22" s="65">
-        <f>M2*H21/R2</f>
-        <v>32.68540033999092</v>
-      </c>
-      <c r="I22" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="M22" s="23">
-        <f>(H6/H7)*H14/2</f>
-        <v>9.1248861612296661</v>
-      </c>
-      <c r="N22" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="62"/>
-      <c r="R22" s="62"/>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
-    </row>
-    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="s">
-        <v>205</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="C23" s="65">
-        <f>C21*C12/(C20*C16)</f>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="D23" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="60" t="s">
-        <v>312</v>
-      </c>
-      <c r="H23" s="65">
-        <f>H22-H14</f>
-        <v>19.505009218214738</v>
-      </c>
-      <c r="I23" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="61" t="s">
-        <v>325</v>
-      </c>
-      <c r="L23" s="62" t="s">
-        <v>267</v>
-      </c>
-      <c r="M23" s="74">
-        <f>H21+M22*2</f>
-        <v>267.94783809804039</v>
-      </c>
-      <c r="N23" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-    </row>
-    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="C24" s="102">
-        <f>V15*C13*C22/(1+V16*C14*C23)</f>
-        <v>0.9030649477012892</v>
-      </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="G24" s="60" t="s">
-        <v>313</v>
-      </c>
-      <c r="H24" s="65">
-        <f>(H23+H14)*H20/2</f>
-        <v>326.85400339990917</v>
-      </c>
-      <c r="I24" s="60" t="s">
-        <v>314</v>
-      </c>
-      <c r="J24" s="60"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="76"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="62"/>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-    </row>
-    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
-        <v>328</v>
-      </c>
-      <c r="B25" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="C25" s="102">
-        <f>C24*C17*M2/2</f>
-        <v>0.99297177075985155</v>
-      </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="G25" s="60" t="s">
-        <v>315</v>
-      </c>
-      <c r="H25" s="82">
-        <f>H24*H2</f>
-        <v>196.11240203994549</v>
-      </c>
-      <c r="I25" s="60" t="s">
-        <v>314</v>
-      </c>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
-    </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
-        <v>349</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>351</v>
-      </c>
-      <c r="C26" s="126">
-        <f>4*C24/M2*(COS(M2*C17/2))</f>
-        <v>0.52200645161955517</v>
-      </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="61"/>
-      <c r="T26" s="61"/>
-    </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
-        <v>350</v>
-      </c>
-      <c r="B27" s="62" t="s">
-        <v>352</v>
-      </c>
-      <c r="C27" s="102">
-        <f>C26*2/M2</f>
-        <v>0.33231962878418064</v>
-      </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="107" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
-    </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="B28" s="62"/>
-      <c r="C28" s="102">
-        <f>C24*C17*R9*R10*M2/R3/1000</f>
-        <v>1.9998309272554275</v>
-      </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q28" s="128" t="s">
-        <v>355</v>
-      </c>
-      <c r="R28" s="129">
-        <f>C25</f>
-        <v>0.99297177075985155</v>
-      </c>
-      <c r="S28" s="128"/>
-      <c r="T28" s="128"/>
-    </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="61" t="s">
-        <v>354</v>
-      </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="102">
-        <f>2*C26*R9*R10/R3/1000</f>
-        <v>1.0513135185875508</v>
-      </c>
-      <c r="P29" s="127" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="130" t="s">
-        <v>22</v>
-      </c>
-      <c r="R29" s="131">
-        <f>R2*M15*C9*M19/(M2*R9)</f>
-        <v>29.859548249533173</v>
-      </c>
-      <c r="S29" s="130" t="s">
-        <v>23</v>
-      </c>
-      <c r="T29" s="130"/>
-    </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P30" s="93" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q30" s="128"/>
-      <c r="R30" s="128"/>
-      <c r="S30" s="128"/>
-      <c r="T30" s="128"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="P31" s="91" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="92"/>
-      <c r="T31" s="92"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q29" s="61" t="s">
+        <v>379</v>
+      </c>
+      <c r="R29" s="81">
+        <f>R24*M7/1000</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="61" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="101"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="60" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q30" s="61" t="s">
+        <v>380</v>
+      </c>
+      <c r="R30" s="81">
+        <f>R25*M6/1000</f>
+        <v>7.3417602193471687</v>
+      </c>
+      <c r="S30" s="61" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P31" s="60"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="81"/>
+      <c r="S31" s="61"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="P32" s="104" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q32" s="105"/>
-      <c r="R32" s="121">
-        <f>M19*M17</f>
-        <v>649.86469631032458</v>
-      </c>
-      <c r="S32" s="105"/>
-      <c r="T32" s="105"/>
-    </row>
-    <row r="33" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P33" s="104" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q33" s="105"/>
-      <c r="R33" s="121">
-        <f>R32*C4*C6</f>
-        <v>7798.3763557238944</v>
-      </c>
-      <c r="S33" s="105"/>
-      <c r="T33" s="105"/>
-    </row>
-    <row r="34" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P34" s="59"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="60"/>
-    </row>
-    <row r="35" spans="16:20" x14ac:dyDescent="0.2">
-      <c r="P35" s="59"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60"/>
-      <c r="T35" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="81"/>
+      <c r="S32" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="P27:T27"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="P11:T11"/>
-    <mergeCell ref="T14:T16"/>
+  <mergeCells count="14">
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="J17:J20"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="P22:T22"/>
+    <mergeCell ref="F12:J12"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="P1:T1"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="W20" r:id="rId1"/>
+    <hyperlink ref="W21" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6139,181 +6505,181 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="77" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="77" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="79">
+      <c r="A2" s="78">
         <v>0</v>
       </c>
-      <c r="B2" s="78">
+      <c r="B2" s="77">
         <v>0.96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="79">
+      <c r="A3" s="78">
         <v>-41668.491999999998</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="77">
         <v>0.90764053175022497</v>
       </c>
       <c r="C3">
         <f>(B2-B3)/(A2-A3)</f>
         <v>1.256572190080097E-6</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="79">
         <f>1/(C3/'SH1'!M5)</f>
         <v>1.0000516245070639</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="79">
+      <c r="A4" s="78">
         <v>-83336.985000000001</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="77">
         <v>0.85527835989871304</v>
       </c>
       <c r="C4">
         <f>(B3-B4)/(A3-A4)</f>
         <v>1.2566370435213947E-6</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="79">
         <f>1/(C4/'SH1'!M5)</f>
         <v>1.0000000131132576</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="79">
+      <c r="A5" s="78">
         <v>-125005.477</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="77">
         <v>0.802916188047201</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C10" si="0">(B4-B5)/(A4-A5)</f>
         <v>1.2566370736793652E-6</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="79">
         <f>1/(C5/'SH1'!M5)</f>
         <v>0.9999999891143071</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="79">
+      <c r="A6" s="78">
         <v>-166673.97</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="77">
         <v>0.75055401619568896</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
         <v>1.2566370435213972E-6</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="79">
         <f>1/(C6/'SH1'!M5)</f>
         <v>1.0000000131132556</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="79">
+      <c r="A7" s="78">
         <v>-208342.462</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="77">
         <v>0.69819184434417803</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>1.2566370736793387E-6</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="79">
         <f>1/(C7/'SH1'!M5)</f>
         <v>0.99999998911432819</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="79">
+      <c r="A8" s="78">
         <v>-250010.954</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="77">
         <v>0.64582967249266598</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
         <v>1.2566370736793652E-6</v>
       </c>
-      <c r="D8" s="80">
+      <c r="D8" s="79">
         <f>1/(C8/'SH1'!M5)</f>
         <v>0.9999999891143071</v>
       </c>
-      <c r="F8" s="81"/>
+      <c r="F8" s="80"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="79">
+      <c r="A9" s="78">
         <v>-291679.44699999999</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="77">
         <v>0.59346750064115605</v>
       </c>
       <c r="C9">
         <f>(B8-B9)/(A8-A9)</f>
         <v>1.2566370435213471E-6</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="79">
         <f>1/(C9/'SH1'!M5)</f>
         <v>1.0000000131132956</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="79">
+      <c r="A10" s="78">
         <v>-333347.93900000001</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="77">
         <v>0.54110532878964401</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>1.2566370736793643E-6</v>
       </c>
-      <c r="D10" s="80">
+      <c r="D10" s="79">
         <f>1/(C10/'SH1'!M5)</f>
         <v>0.99999998911430776</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
+      <c r="A11" s="78"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="78"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
+      <c r="A13" s="78"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
+      <c r="A14" s="78"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="78"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
+      <c r="A16" s="78"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="78"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
+      <c r="A18" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7056,12 +7422,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="115" t="s">
+      <c r="F7" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -7322,35 +7688,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="129" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119" t="s">
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="116" t="s">
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="126" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="118"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="128"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7572,7 +7938,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="120" t="s">
+      <c r="J5" s="130" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -7639,7 +8005,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="120"/>
+      <c r="J6" s="130"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -7866,20 +8232,20 @@
       <c r="E10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="119" t="s">
+      <c r="F10" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119" t="s">
+      <c r="G10" s="129"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="129" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="119"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="129"/>
+      <c r="O10" s="129"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -7944,7 +8310,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="120" t="s">
+      <c r="O11" s="130" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -8011,7 +8377,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="120"/>
+      <c r="O12" s="130"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -8077,7 +8443,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="120"/>
+      <c r="O13" s="130"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -8242,13 +8608,13 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="119" t="s">
+      <c r="F17" s="129" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="119"/>
-      <c r="H17" s="119"/>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="129"/>
       <c r="K17" s="29" t="s">
         <v>140</v>
       </c>
@@ -8487,13 +8853,13 @@
         <v>15</v>
       </c>
       <c r="J23" s="46"/>
-      <c r="K23" s="119" t="s">
+      <c r="K23" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="119"/>
-      <c r="M23" s="119"/>
-      <c r="N23" s="119"/>
-      <c r="O23" s="119"/>
+      <c r="L23" s="129"/>
+      <c r="M23" s="129"/>
+      <c r="N23" s="129"/>
+      <c r="O23" s="129"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="44"/>

</xml_diff>

<commit_message>
Design file V1.1 is almost finished. A new design methodology is being developed (V1.2) after talking to Reza. He has some good points :) After the second version, optimization will be applied for the sake of PEMD conference paper.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="403">
   <si>
     <t>Power factor</t>
   </si>
@@ -3170,9 +3170,6 @@
     <t>Verification</t>
   </si>
   <si>
-    <t>Mass</t>
-  </si>
-  <si>
     <t>Power density</t>
   </si>
   <si>
@@ -3227,12 +3224,6 @@
     <t>Outer diemeter</t>
   </si>
   <si>
-    <t>Iphm x Ephm</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Peak flux density</t>
   </si>
   <si>
@@ -3380,9 +3371,6 @@
   </si>
   <si>
     <t>Magnet volume</t>
-  </si>
-  <si>
-    <t>Iron volume</t>
   </si>
   <si>
     <t>Copper volume</t>
@@ -3439,22 +3427,6 @@
         <family val="1"/>
         <charset val="162"/>
       </rPr>
-      <t>c</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
       <t>cu</t>
     </r>
   </si>
@@ -3644,6 +3616,237 @@
   </si>
   <si>
     <t>kg</t>
+  </si>
+  <si>
+    <r>
+      <t>pd</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>Output power (module)</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>outm</t>
+    </r>
+  </si>
+  <si>
+    <t>Output power (total)</t>
+  </si>
+  <si>
+    <t>Copper loss (module)</t>
+  </si>
+  <si>
+    <t>Copper loss (total)</t>
+  </si>
+  <si>
+    <t>Resistance and copper loss</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu-m</t>
+    </r>
+  </si>
+  <si>
+    <t>Stator core volume</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cs</t>
+    </r>
+  </si>
+  <si>
+    <t>Rotor core volume</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cr</t>
+    </r>
+  </si>
+  <si>
+    <t>Total mass</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>total</t>
+    </r>
+  </si>
+  <si>
+    <t>Stator back core flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>sy</t>
+    </r>
+  </si>
+  <si>
+    <t>Stator teeth flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>st</t>
+    </r>
+  </si>
+  <si>
+    <t>Rotor back core flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>ry</t>
+    </r>
+  </si>
+  <si>
+    <t>Coging torque</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cg</t>
+    </r>
+  </si>
+  <si>
+    <t>Stator slot fill factor</t>
   </si>
 </sst>
 </file>
@@ -3859,18 +4062,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3884,6 +4075,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3990,7 +4193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4241,64 +4444,32 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="170" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4356,17 +4527,63 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4849,10 +5066,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4868,14 +5085,14 @@
     <col min="9" max="9" width="7" style="69" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="70" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" style="70" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="70" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="70" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" style="70" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.140625" style="70" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="70" bestFit="1" customWidth="1"/>
@@ -4883,34 +5100,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
       <c r="J1" s="63"/>
-      <c r="K1" s="113" t="s">
+      <c r="K1" s="101" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
       <c r="O1" s="63"/>
-      <c r="P1" s="113" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
+      <c r="P1" s="101" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="101"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
@@ -5159,16 +5376,16 @@
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="60" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="L6" s="61" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="M6" s="61">
         <v>8.9600000000000009</v>
       </c>
       <c r="N6" s="61" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="O6" s="60"/>
       <c r="P6" s="58" t="s">
@@ -5214,14 +5431,16 @@
       </c>
       <c r="J7" s="59"/>
       <c r="K7" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="L7" s="61" t="s">
         <v>369</v>
       </c>
-      <c r="L7" s="61" t="s">
-        <v>374</v>
-      </c>
-      <c r="M7" s="61"/>
+      <c r="M7" s="61">
+        <v>7.6</v>
+      </c>
       <c r="N7" s="61" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="O7" s="60"/>
       <c r="P7" s="58" t="s">
@@ -5253,24 +5472,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="62"/>
-      <c r="F8" s="119" t="s">
+      <c r="F8" s="107" t="s">
         <v>246</v>
       </c>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="121"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="109"/>
       <c r="K8" s="60" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="L8" s="61" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="M8" s="61">
         <v>7.4</v>
       </c>
       <c r="N8" s="61" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="O8" s="60"/>
       <c r="P8" s="58" t="s">
@@ -5357,7 +5576,10 @@
       <c r="J10" s="59"/>
       <c r="K10" s="60"/>
       <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
+      <c r="M10" s="61">
+        <f>H3*1000*M2*R9/H5/1000000</f>
+        <v>5.5169762227105927</v>
+      </c>
       <c r="N10" s="61"/>
       <c r="O10" s="60"/>
       <c r="P10" s="58" t="s">
@@ -5375,7 +5597,7 @@
       </c>
       <c r="T10" s="61"/>
       <c r="U10" s="70" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="V10" s="70">
         <f>M18*SQRT(3)*4</f>
@@ -5413,34 +5635,34 @@
       <c r="T11" s="61"/>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="102" t="s">
         <v>269</v>
       </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="119" t="s">
+      <c r="B12" s="102"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="107" t="s">
         <v>280</v>
       </c>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="121"/>
-      <c r="K12" s="115" t="s">
+      <c r="G12" s="108"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="114" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q12" s="114"/>
-      <c r="R12" s="114"/>
-      <c r="S12" s="114"/>
-      <c r="T12" s="114"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="104"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="102" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="102"/>
+      <c r="T12" s="102"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="60" t="s">
@@ -5455,9 +5677,7 @@
       <c r="D13" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>178</v>
-      </c>
+      <c r="E13" s="62"/>
       <c r="F13" s="60" t="s">
         <v>92</v>
       </c>
@@ -5484,7 +5704,7 @@
       <c r="N13" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="112" t="s">
+      <c r="O13" s="100" t="s">
         <v>179</v>
       </c>
       <c r="P13" s="74" t="s">
@@ -5520,7 +5740,7 @@
         <v>295</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H14" s="81">
         <f>C25/H6</f>
@@ -5545,12 +5765,12 @@
       </c>
       <c r="O14" s="62"/>
       <c r="P14" s="60" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q14" s="61" t="s">
-        <v>338</v>
-      </c>
-      <c r="R14" s="101">
+        <v>335</v>
+      </c>
+      <c r="R14" s="98">
         <f>2*SQRT(M20/(M2*H5))</f>
         <v>1.4425038006176998</v>
       </c>
@@ -5591,7 +5811,7 @@
         <v>25</v>
       </c>
       <c r="L15" s="59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M15" s="59">
         <f>R3*C7/120</f>
@@ -5602,10 +5822,10 @@
       </c>
       <c r="O15" s="60"/>
       <c r="P15" s="60" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q15" s="61" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="R15" s="61">
         <v>14</v>
@@ -5613,7 +5833,7 @@
       <c r="S15" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="T15" s="122" t="s">
+      <c r="T15" s="110" t="s">
         <v>178</v>
       </c>
     </row>
@@ -5649,31 +5869,31 @@
       <c r="K16" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="93" t="s">
+      <c r="L16" s="90" t="s">
         <v>298</v>
       </c>
-      <c r="M16" s="93">
+      <c r="M16" s="90">
         <v>60</v>
       </c>
-      <c r="N16" s="93" t="s">
+      <c r="N16" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="93" t="s">
+      <c r="O16" s="90" t="s">
         <v>178</v>
       </c>
       <c r="P16" s="60" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="Q16" s="61" t="s">
-        <v>338</v>
-      </c>
-      <c r="R16" s="106">
+        <v>335</v>
+      </c>
+      <c r="R16" s="99">
         <v>1.6281399999999999</v>
       </c>
       <c r="S16" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T16" s="123"/>
+      <c r="T16" s="111"/>
       <c r="U16" s="70" t="s">
         <v>288</v>
       </c>
@@ -5709,7 +5929,7 @@
       <c r="I17" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="118" t="s">
+      <c r="J17" s="106" t="s">
         <v>178</v>
       </c>
       <c r="K17" s="58" t="s">
@@ -5727,10 +5947,10 @@
       </c>
       <c r="O17" s="62"/>
       <c r="P17" s="60" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Q17" s="59" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="R17" s="61">
         <v>8.282</v>
@@ -5738,7 +5958,7 @@
       <c r="S17" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="T17" s="124"/>
+      <c r="T17" s="112"/>
       <c r="U17" s="70" t="s">
         <v>221</v>
       </c>
@@ -5774,26 +5994,26 @@
       <c r="I18" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="118"/>
-      <c r="K18" s="94" t="s">
+      <c r="J18" s="106"/>
+      <c r="K18" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="L18" s="95" t="s">
+      <c r="L18" s="92" t="s">
         <v>302</v>
       </c>
-      <c r="M18" s="96">
+      <c r="M18" s="93">
         <f>4.44*M17*M15*M14*M13/1000</f>
         <v>99.41207535328985</v>
       </c>
-      <c r="N18" s="95" t="s">
+      <c r="N18" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="97"/>
+      <c r="O18" s="94"/>
       <c r="P18" s="60" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="Q18" s="61" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="R18" s="81">
         <f>2*R10*V18+2*H13</f>
@@ -5804,7 +6024,7 @@
       </c>
       <c r="T18" s="61"/>
       <c r="U18" s="70" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V18" s="70">
         <v>1.1000000000000001</v>
@@ -5837,9 +6057,9 @@
       <c r="I19" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="118"/>
+      <c r="J19" s="106"/>
       <c r="K19" s="58" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L19" s="59" t="s">
         <v>304</v>
@@ -5853,10 +6073,10 @@
       </c>
       <c r="O19" s="60"/>
       <c r="P19" s="60" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q19" s="61" t="s">
         <v>343</v>
-      </c>
-      <c r="Q19" s="61" t="s">
-        <v>346</v>
       </c>
       <c r="R19" s="81">
         <f>R18*M17/1000</f>
@@ -5894,33 +6114,33 @@
       <c r="I20" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="118"/>
-      <c r="K20" s="97" t="s">
+      <c r="J20" s="106"/>
+      <c r="K20" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="95" t="s">
+      <c r="L20" s="92" t="s">
         <v>316</v>
       </c>
-      <c r="M20" s="98">
+      <c r="M20" s="95">
         <f>H5*H26/(2*M16)</f>
         <v>6.5370800679981835</v>
       </c>
-      <c r="N20" s="99" t="s">
+      <c r="N20" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="99"/>
+      <c r="O20" s="96"/>
       <c r="P20" s="60" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="Q20" s="61" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="R20" s="81">
         <f>R17*R19/1000</f>
         <v>0.27162691034686004</v>
       </c>
       <c r="S20" s="59" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="T20" s="61"/>
       <c r="U20" s="70" t="s">
@@ -5929,8 +6149,8 @@
       <c r="V20" s="70" t="s">
         <v>293</v>
       </c>
-      <c r="W20" s="135" t="s">
-        <v>331</v>
+      <c r="W20" s="123" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5951,27 +6171,36 @@
       <c r="F21" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="G21" s="93" t="s">
+      <c r="G21" s="90" t="s">
         <v>311</v>
       </c>
-      <c r="H21" s="93">
+      <c r="H21" s="90">
         <v>20</v>
       </c>
-      <c r="I21" s="93" t="s">
+      <c r="I21" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="J21" s="93" t="s">
+      <c r="J21" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="100"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="61"/>
-      <c r="S21" s="61"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="97"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="60" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q21" s="61" t="s">
+        <v>387</v>
+      </c>
+      <c r="R21" s="81">
+        <f>R20*M20^2*C6</f>
+        <v>34.82263711952983</v>
+      </c>
+      <c r="S21" s="61" t="s">
+        <v>7</v>
+      </c>
       <c r="T21" s="61"/>
       <c r="U21" s="70" t="s">
         <v>294</v>
@@ -5979,11 +6208,11 @@
       <c r="V21" s="70" t="s">
         <v>289</v>
       </c>
-      <c r="W21" s="135" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W21" s="123" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
         <v>188</v>
       </c>
@@ -6012,25 +6241,28 @@
         <v>80</v>
       </c>
       <c r="J22" s="60"/>
-      <c r="K22" s="114" t="s">
-        <v>319</v>
-      </c>
-      <c r="L22" s="114"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="114"/>
-      <c r="O22" s="114"/>
-      <c r="P22" s="115" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="116"/>
-      <c r="T22" s="117"/>
-      <c r="W22" s="70" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="134"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="135"/>
+      <c r="O22" s="136"/>
+      <c r="P22" s="60" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q22" s="61" t="s">
+        <v>386</v>
+      </c>
+      <c r="R22" s="81">
+        <f>C4*R21</f>
+        <v>139.29054847811932</v>
+      </c>
+      <c r="S22" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="T22" s="61"/>
+      <c r="W22" s="123"/>
+    </row>
+    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
         <v>203</v>
       </c>
@@ -6049,7 +6281,7 @@
         <v>149</v>
       </c>
       <c r="G23" s="59" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H23" s="64">
         <f>M2*H22/R2</f>
@@ -6059,34 +6291,23 @@
         <v>80</v>
       </c>
       <c r="J23" s="60"/>
-      <c r="K23" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="108" t="s">
-        <v>352</v>
-      </c>
-      <c r="M23" s="109">
-        <f>C26</f>
-        <v>0.99297177075985155</v>
-      </c>
-      <c r="N23" s="108" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="108"/>
-      <c r="P23" s="60" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q23" s="61" t="s">
-        <v>361</v>
-      </c>
-      <c r="R23" s="81">
-        <f>C17*R10*C18*M2*(R9-C13)/R3/1000</f>
-        <v>6.6103768836310586</v>
-      </c>
-      <c r="S23" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="T23" s="61"/>
+      <c r="K23" s="103" t="s">
+        <v>351</v>
+      </c>
+      <c r="L23" s="104"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="104"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="102" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q23" s="102"/>
+      <c r="R23" s="102"/>
+      <c r="S23" s="102"/>
+      <c r="T23" s="102"/>
+      <c r="W23" s="70" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
@@ -6117,31 +6338,34 @@
         <v>80</v>
       </c>
       <c r="J24" s="62"/>
-      <c r="K24" s="107" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="110" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" s="111">
-        <f>R2*M16*C9*M20/(M2*R9)</f>
-        <v>29.859548249533173</v>
-      </c>
-      <c r="N24" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="O24" s="110"/>
-      <c r="P24" s="60" t="s">
+      <c r="K24" s="60" t="s">
+        <v>352</v>
+      </c>
+      <c r="L24" s="61" t="s">
+        <v>357</v>
+      </c>
+      <c r="M24" s="81">
+        <f>C17*R10*C18*M2*(R9-C13)/R3/1000</f>
+        <v>6.6103768836310586</v>
+      </c>
+      <c r="N24" s="61" t="s">
         <v>356</v>
       </c>
-      <c r="Q24" s="61" t="s">
-        <v>362</v>
-      </c>
-      <c r="R24" s="81"/>
-      <c r="S24" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="T24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="124" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="125" t="s">
+        <v>349</v>
+      </c>
+      <c r="R24" s="126">
+        <f>C26</f>
+        <v>0.99297177075985155</v>
+      </c>
+      <c r="S24" s="125" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="125"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
@@ -6150,7 +6374,7 @@
       <c r="B25" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="C25" s="101">
+      <c r="C25" s="98">
         <f>V16*C14*C23/(1+V17*C15*C24)</f>
         <v>0.9030649477012892</v>
       </c>
@@ -6170,36 +6394,43 @@
         <v>314</v>
       </c>
       <c r="J25" s="59"/>
-      <c r="K25" s="92" t="s">
-        <v>320</v>
-      </c>
-      <c r="L25" s="108"/>
-      <c r="M25" s="108"/>
-      <c r="N25" s="108"/>
-      <c r="O25" s="108"/>
-      <c r="P25" s="60" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q25" s="61" t="s">
-        <v>363</v>
-      </c>
-      <c r="R25" s="81">
-        <f>R19*C6*C4*(R16/2)^2*M2</f>
-        <v>819.39288162356786</v>
-      </c>
-      <c r="S25" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="T25" s="61"/>
+      <c r="K25" s="70" t="s">
+        <v>388</v>
+      </c>
+      <c r="L25" s="61" t="s">
+        <v>389</v>
+      </c>
+      <c r="M25" s="139">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="O25" s="61"/>
+      <c r="P25" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="128" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="129">
+        <f>R2*M16*C9*M20/(M2*R9)</f>
+        <v>29.859548249533173</v>
+      </c>
+      <c r="S25" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="T25" s="128"/>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>329</v>
-      </c>
-      <c r="C26" s="101">
+        <v>326</v>
+      </c>
+      <c r="C26" s="98">
         <f>C25*C18*M2/2</f>
         <v>0.99297177075985155</v>
       </c>
@@ -6219,81 +6450,92 @@
         <v>314</v>
       </c>
       <c r="J26" s="60"/>
-      <c r="K26" s="90" t="s">
-        <v>321</v>
-      </c>
-      <c r="L26" s="91"/>
-      <c r="M26" s="102"/>
-      <c r="N26" s="91"/>
-      <c r="O26" s="91"/>
-      <c r="P26" s="60" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q26" s="61" t="s">
-        <v>364</v>
-      </c>
-      <c r="R26" s="81">
-        <f>M2*R9*R10/1000</f>
-        <v>63.271226104450712</v>
-      </c>
-      <c r="S26" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="T26" s="61"/>
+      <c r="K26" s="60" t="s">
+        <v>390</v>
+      </c>
+      <c r="L26" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="M26" s="137">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="O26" s="61"/>
+      <c r="P26" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="R26" s="130">
+        <f>M16*C9*M20/(M2*(R16/2)*M16)</f>
+        <v>5.1121333909774558</v>
+      </c>
+      <c r="S26" s="125" t="s">
+        <v>244</v>
+      </c>
+      <c r="T26" s="125"/>
     </row>
     <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="131" t="s">
-        <v>348</v>
-      </c>
-      <c r="B27" s="132" t="s">
-        <v>350</v>
-      </c>
-      <c r="C27" s="133">
+      <c r="A27" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="120" t="s">
+        <v>347</v>
+      </c>
+      <c r="C27" s="121">
         <f>4*C25/M2*(COS(M2*C18/2))</f>
         <v>0.52200645161955517</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
-      <c r="F27" s="115" t="s">
+      <c r="F27" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="103" t="s">
-        <v>326</v>
-      </c>
-      <c r="L27" s="104"/>
-      <c r="M27" s="105">
-        <f>M20*M18</f>
-        <v>649.86469631032458</v>
-      </c>
-      <c r="N27" s="104"/>
-      <c r="O27" s="104"/>
-      <c r="P27" s="60" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q27" s="61" t="s">
-        <v>365</v>
-      </c>
-      <c r="R27" s="81">
-        <f>M2*H29*R10/1000</f>
-        <v>84.472105812205513</v>
-      </c>
-      <c r="S27" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="T27" s="61"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="60" t="s">
+        <v>353</v>
+      </c>
+      <c r="L27" s="61" t="s">
+        <v>358</v>
+      </c>
+      <c r="M27" s="81">
+        <f>R19*C6*C4*(R16/2)^2*M2</f>
+        <v>819.39288162356786</v>
+      </c>
+      <c r="N27" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="O27" s="61"/>
+      <c r="P27" s="131" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q27" s="132" t="s">
+        <v>378</v>
+      </c>
+      <c r="R27" s="133">
+        <f>C2/M29</f>
+        <v>94.705819430916407</v>
+      </c>
+      <c r="S27" s="132" t="s">
+        <v>379</v>
+      </c>
+      <c r="T27" s="132"/>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="131" t="s">
-        <v>349</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>351</v>
-      </c>
-      <c r="C28" s="134">
+      <c r="A28" s="119" t="s">
+        <v>346</v>
+      </c>
+      <c r="B28" s="120" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="122">
         <f>C27*2/M2</f>
         <v>0.33231962878418064</v>
       </c>
@@ -6313,38 +6555,42 @@
         <v>80</v>
       </c>
       <c r="J28" s="60"/>
-      <c r="K28" s="103" t="s">
-        <v>327</v>
-      </c>
-      <c r="L28" s="104"/>
-      <c r="M28" s="105">
-        <f>M27*C4*C6</f>
-        <v>7798.3763557238944</v>
-      </c>
-      <c r="N28" s="104"/>
-      <c r="O28" s="104"/>
-      <c r="P28" s="60" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q28" s="61" t="s">
-        <v>378</v>
-      </c>
-      <c r="R28" s="81">
-        <f>R23*M8</f>
-        <v>48.916788938869836</v>
-      </c>
-      <c r="S28" s="61" t="s">
+      <c r="K28" s="60" t="s">
+        <v>354</v>
+      </c>
+      <c r="L28" s="61" t="s">
+        <v>359</v>
+      </c>
+      <c r="M28" s="81">
+        <f>M2*R9*R10/1000</f>
+        <v>63.271226104450712</v>
+      </c>
+      <c r="N28" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="O28" s="61"/>
+      <c r="P28" s="131" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q28" s="132" t="s">
         <v>381</v>
       </c>
+      <c r="R28" s="133">
+        <f>M20*M18</f>
+        <v>649.86469631032458</v>
+      </c>
+      <c r="S28" s="132" t="s">
+        <v>7</v>
+      </c>
+      <c r="T28" s="132"/>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="60" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G29" s="61" t="s">
         <v>267</v>
@@ -6357,71 +6603,214 @@
         <v>80</v>
       </c>
       <c r="J29" s="60"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="60" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q29" s="61" t="s">
-        <v>379</v>
-      </c>
-      <c r="R29" s="81">
-        <f>R24*M7/1000</f>
-        <v>0</v>
-      </c>
-      <c r="S29" s="61" t="s">
-        <v>381</v>
-      </c>
+      <c r="K29" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L29" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="M29" s="137">
+        <f>M2*H29*R10/1000</f>
+        <v>84.472105812205513</v>
+      </c>
+      <c r="N29" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="O29" s="60"/>
+      <c r="P29" s="131" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q29" s="132" t="s">
+        <v>239</v>
+      </c>
+      <c r="R29" s="133">
+        <f>R28*C4*C6</f>
+        <v>7798.3763557238944</v>
+      </c>
+      <c r="S29" s="132" t="s">
+        <v>7</v>
+      </c>
+      <c r="T29" s="132"/>
     </row>
     <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
       <c r="B30" s="61"/>
-      <c r="C30" s="101"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="60" t="s">
+      <c r="C30" s="98"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="L30" s="61" t="s">
+        <v>373</v>
+      </c>
+      <c r="M30" s="138">
+        <f>M24*M8</f>
+        <v>48.916788938869836</v>
+      </c>
+      <c r="N30" s="61" t="s">
+        <v>376</v>
+      </c>
+      <c r="O30" s="60"/>
+      <c r="P30" s="131" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q30" s="132" t="s">
+        <v>395</v>
+      </c>
+      <c r="R30" s="132"/>
+      <c r="S30" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="T30" s="132"/>
+    </row>
+    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="L31" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="M31" s="138">
+        <f>M26*M7/1000</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="61" t="s">
         <v>377</v>
       </c>
-      <c r="Q30" s="61" t="s">
-        <v>380</v>
-      </c>
-      <c r="R30" s="81">
-        <f>R25*M6/1000</f>
+      <c r="O31" s="60"/>
+      <c r="P31" s="131" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q31" s="132" t="s">
+        <v>397</v>
+      </c>
+      <c r="R31" s="132"/>
+      <c r="S31" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="T31" s="132"/>
+    </row>
+    <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="140" t="s">
+        <v>372</v>
+      </c>
+      <c r="L32" s="141" t="s">
+        <v>375</v>
+      </c>
+      <c r="M32" s="142">
+        <f>M27*M6/1000</f>
         <v>7.3417602193471687</v>
       </c>
-      <c r="S30" s="61" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P31" s="60"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="81"/>
-      <c r="S31" s="61"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="P32" s="60"/>
-      <c r="Q32" s="61"/>
-      <c r="R32" s="81"/>
-      <c r="S32" s="61"/>
+      <c r="N32" s="141" t="s">
+        <v>377</v>
+      </c>
+      <c r="P32" s="131" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q32" s="132" t="s">
+        <v>399</v>
+      </c>
+      <c r="R32" s="132"/>
+      <c r="S32" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="T32" s="125"/>
+    </row>
+    <row r="33" spans="1:20" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="60" t="s">
+        <v>392</v>
+      </c>
+      <c r="L33" s="60" t="s">
+        <v>393</v>
+      </c>
+      <c r="M33" s="61"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="143"/>
+      <c r="P33" s="124" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q33" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="R33" s="125"/>
+      <c r="S33" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="T33" s="125"/>
+    </row>
+    <row r="34" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P34" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q34" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="R34" s="59"/>
+      <c r="S34" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="T34" s="60"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P44" s="60"/>
+      <c r="Q44" s="61"/>
+      <c r="R44" s="81"/>
+      <c r="S44" s="61"/>
+      <c r="T44" s="60"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P45" s="60"/>
+      <c r="Q45" s="61"/>
+      <c r="R45" s="81"/>
+      <c r="S45" s="61"/>
+      <c r="T45" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="P23:T23"/>
     <mergeCell ref="J17:J20"/>
     <mergeCell ref="K12:O12"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="P12:T12"/>
     <mergeCell ref="T15:T17"/>
-    <mergeCell ref="P22:T22"/>
+    <mergeCell ref="K23:O23"/>
     <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F27:J27"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
@@ -7422,12 +7811,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="125" t="s">
+      <c r="F7" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -7688,35 +8077,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129" t="s">
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="126" t="s">
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="114" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="128"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="116"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7938,7 +8327,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="130" t="s">
+      <c r="J5" s="118" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -8005,7 +8394,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="130"/>
+      <c r="J6" s="118"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -8232,20 +8621,20 @@
       <c r="E10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="129" t="s">
+      <c r="F10" s="117" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="129"/>
-      <c r="H10" s="129"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="129" t="s">
+      <c r="G10" s="117"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="117" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
-      <c r="O10" s="129"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="117"/>
+      <c r="N10" s="117"/>
+      <c r="O10" s="117"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -8310,7 +8699,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="130" t="s">
+      <c r="O11" s="118" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -8377,7 +8766,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="130"/>
+      <c r="O12" s="118"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -8443,7 +8832,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="130"/>
+      <c r="O13" s="118"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -8608,13 +8997,13 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="129" t="s">
+      <c r="F17" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="129"/>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
       <c r="K17" s="29" t="s">
         <v>140</v>
       </c>
@@ -8853,13 +9242,13 @@
         <v>15</v>
       </c>
       <c r="J23" s="46"/>
-      <c r="K23" s="129" t="s">
+      <c r="K23" s="117" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="129"/>
-      <c r="M23" s="129"/>
-      <c r="N23" s="129"/>
-      <c r="O23" s="129"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="117"/>
+      <c r="O23" s="117"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="44"/>

</xml_diff>

<commit_message>
New design procedure start.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.1.xlsx
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="415">
   <si>
     <t>Power factor</t>
   </si>
@@ -2321,8 +2321,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>ρ</t>
+    <t>Ωm</t>
+  </si>
+  <si>
+    <r>
+      <t>η</t>
     </r>
     <r>
       <rPr>
@@ -2333,58 +2336,7 @@
         <family val="1"/>
         <charset val="162"/>
       </rPr>
-      <t>cu</t>
-    </r>
-  </si>
-  <si>
-    <t>Ωm</t>
-  </si>
-  <si>
-    <r>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>cu</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>η</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
       <t>d</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>0</t>
     </r>
   </si>
   <si>
@@ -3271,25 +3223,6 @@
   </si>
   <si>
     <t>AWG</t>
-  </si>
-  <si>
-    <t>Wire specific resiatance</t>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>sp</t>
-    </r>
   </si>
   <si>
     <t>Mean length turn</t>
@@ -3612,9 +3545,6 @@
     </r>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -3847,6 +3777,184 @@
   </si>
   <si>
     <t>Stator slot fill factor</t>
+  </si>
+  <si>
+    <t>mx</t>
+  </si>
+  <si>
+    <t>Minimum outer diameter</t>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>osm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>Copper temp coeff (20 C)</t>
+  </si>
+  <si>
+    <r>
+      <t>1/</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>C</t>
+    </r>
+  </si>
+  <si>
+    <t>Copper resistivity (70 C)</t>
+  </si>
+  <si>
+    <t>Copper resistivity (20 C)</t>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>Area of single wire</t>
+  </si>
+  <si>
+    <t>Aw</t>
+  </si>
+  <si>
+    <t>Slot area (with wedge)</t>
+  </si>
+  <si>
+    <t>Stator iron mass</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>sc</t>
+    </r>
+  </si>
+  <si>
+    <t>Rotor inner diameter</t>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>ir</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3862,7 +3970,7 @@
     <numFmt numFmtId="169" formatCode="0.0000000000"/>
     <numFmt numFmtId="170" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4016,8 +4124,32 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4081,12 +4213,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4193,7 +4319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4473,60 +4599,6 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4564,26 +4636,95 @@
     <xf numFmtId="2" fontId="14" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5066,10 +5207,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5086,48 +5227,48 @@
     <col min="10" max="10" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" style="70" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="70" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="69" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="70" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" style="70" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="70" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" style="70" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" style="70" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" style="70" customWidth="1"/>
     <col min="22" max="22" width="9" style="70" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="133" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101" t="s">
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
       <c r="J1" s="63"/>
-      <c r="K1" s="101" t="s">
+      <c r="K1" s="133" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
       <c r="O1" s="63"/>
-      <c r="P1" s="101" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
+      <c r="P1" s="133" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
@@ -5171,7 +5312,7 @@
         <v>2</v>
       </c>
       <c r="Q2" s="59" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="R2" s="59">
         <f>C4*C8*C6</f>
@@ -5210,16 +5351,16 @@
       </c>
       <c r="J3" s="59"/>
       <c r="K3" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" s="59" t="s">
-        <v>251</v>
+        <v>404</v>
+      </c>
+      <c r="L3" s="121" t="s">
+        <v>405</v>
       </c>
       <c r="M3" s="65">
         <v>1.7E-8</v>
       </c>
       <c r="N3" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O3" s="59"/>
       <c r="P3" s="58" t="s">
@@ -5252,7 +5393,7 @@
       </c>
       <c r="E4" s="59"/>
       <c r="F4" s="58" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G4" s="59" t="s">
         <v>248</v>
@@ -5267,8 +5408,8 @@
       <c r="K4" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="L4" s="59" t="s">
-        <v>253</v>
+      <c r="L4" s="121" t="s">
+        <v>406</v>
       </c>
       <c r="M4" s="65">
         <v>1.2566289999999999E-6</v>
@@ -5291,6 +5432,10 @@
         <v>73</v>
       </c>
       <c r="T4" s="66"/>
+      <c r="U4" s="70">
+        <f>M3*R19/((R16/2)^2*M2)*1000000*4</f>
+        <v>1.0712062726797149</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
@@ -5322,8 +5467,8 @@
       <c r="K5" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="L5" s="59" t="s">
-        <v>255</v>
+      <c r="L5" s="121" t="s">
+        <v>407</v>
       </c>
       <c r="M5" s="65">
         <f>4*M2*0.0000001</f>
@@ -5337,7 +5482,7 @@
         <v>59</v>
       </c>
       <c r="Q5" s="59" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="R5" s="64">
         <f>C2/(C7*2*M2/60)</f>
@@ -5376,30 +5521,30 @@
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="60" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="L6" s="61" t="s">
-        <v>367</v>
-      </c>
-      <c r="M6" s="61">
+        <v>362</v>
+      </c>
+      <c r="M6" s="81">
         <v>8.9600000000000009</v>
       </c>
       <c r="N6" s="61" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="O6" s="60"/>
       <c r="P6" s="58" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Q6" s="59" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="R6" s="67">
         <f>R5/(2*R4)*0.001</f>
         <v>3.174603174603175E-3</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="T6" s="58"/>
     </row>
@@ -5418,10 +5563,10 @@
       </c>
       <c r="E7" s="62"/>
       <c r="F7" s="58" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H7" s="59">
         <v>1.3</v>
@@ -5431,30 +5576,30 @@
       </c>
       <c r="J7" s="59"/>
       <c r="K7" s="60" t="s">
+        <v>359</v>
+      </c>
+      <c r="L7" s="61" t="s">
         <v>364</v>
       </c>
-      <c r="L7" s="61" t="s">
-        <v>369</v>
-      </c>
-      <c r="M7" s="61">
-        <v>7.6</v>
+      <c r="M7" s="81">
+        <v>7.65</v>
       </c>
       <c r="N7" s="61" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="O7" s="60"/>
       <c r="P7" s="58" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Q7" s="59" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="R7" s="67">
         <f>R6*4/M2</f>
         <v>4.042030305365242E-3</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="T7" s="62"/>
     </row>
@@ -5472,24 +5617,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="62"/>
-      <c r="F8" s="107" t="s">
+      <c r="F8" s="136" t="s">
         <v>246</v>
       </c>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="109"/>
+      <c r="G8" s="137"/>
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="138"/>
       <c r="K8" s="60" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="L8" s="61" t="s">
-        <v>368</v>
-      </c>
-      <c r="M8" s="61">
+        <v>363</v>
+      </c>
+      <c r="M8" s="81">
         <v>7.4</v>
       </c>
       <c r="N8" s="61" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="O8" s="60"/>
       <c r="P8" s="58" t="s">
@@ -5508,7 +5653,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>98</v>
       </c>
@@ -5535,16 +5680,24 @@
         <v>51</v>
       </c>
       <c r="J9" s="59"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
+      <c r="K9" s="60" t="s">
+        <v>401</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>400</v>
+      </c>
+      <c r="M9" s="69">
+        <v>4.0410000000000003E-3</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>402</v>
+      </c>
       <c r="O9" s="60"/>
       <c r="P9" s="58" t="s">
         <v>78</v>
       </c>
       <c r="Q9" s="59" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="R9" s="72">
         <f>1000*(R7/R8)^(1/3)</f>
@@ -5574,19 +5727,25 @@
         <v>15</v>
       </c>
       <c r="J10" s="59"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61">
-        <f>H3*1000*M2*R9/H5/1000000</f>
-        <v>5.5169762227105927</v>
-      </c>
-      <c r="N10" s="61"/>
+      <c r="K10" s="60" t="s">
+        <v>403</v>
+      </c>
+      <c r="L10" s="121" t="s">
+        <v>405</v>
+      </c>
+      <c r="M10" s="122">
+        <f>(M9*(70-20)+1)*M3</f>
+        <v>2.0434850000000002E-8</v>
+      </c>
+      <c r="N10" s="59" t="s">
+        <v>251</v>
+      </c>
       <c r="O10" s="60"/>
       <c r="P10" s="58" t="s">
         <v>81</v>
       </c>
       <c r="Q10" s="61" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R10" s="73">
         <f>R9*R8</f>
@@ -5597,7 +5756,7 @@
       </c>
       <c r="T10" s="61"/>
       <c r="U10" s="70" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="V10" s="70">
         <f>M18*SQRT(3)*4</f>
@@ -5614,7 +5773,7 @@
         <v>53</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H11" s="59">
         <v>98</v>
@@ -5628,48 +5787,57 @@
       <c r="M11" s="59"/>
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="61"/>
+      <c r="P11" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q11" s="59" t="s">
+        <v>414</v>
+      </c>
+      <c r="R11" s="73">
+        <f>75</f>
+        <v>75</v>
+      </c>
+      <c r="S11" s="61" t="s">
+        <v>80</v>
+      </c>
       <c r="T11" s="61"/>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102" t="s">
-        <v>269</v>
-      </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="102"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="107" t="s">
-        <v>280</v>
-      </c>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="109"/>
-      <c r="K12" s="103" t="s">
-        <v>317</v>
-      </c>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="105"/>
-      <c r="P12" s="102" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="102"/>
-      <c r="S12" s="102"/>
-      <c r="T12" s="102"/>
+      <c r="A12" s="134" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="134"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="136" t="s">
+        <v>277</v>
+      </c>
+      <c r="G12" s="137"/>
+      <c r="H12" s="137"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="130" t="s">
+        <v>314</v>
+      </c>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="131"/>
+      <c r="O12" s="132"/>
+      <c r="P12" s="134" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q12" s="134"/>
+      <c r="R12" s="134"/>
+      <c r="S12" s="134"/>
+      <c r="T12" s="134"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="60" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C13" s="59">
         <v>1</v>
@@ -5682,7 +5850,7 @@
         <v>92</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H13" s="73">
         <f>M2*R9/R2</f>
@@ -5696,7 +5864,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="59" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="M13" s="59">
         <v>0.93300000000000005</v>
@@ -5727,7 +5895,7 @@
         <v>207</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C14" s="64">
         <v>1.25</v>
@@ -5737,10 +5905,10 @@
       </c>
       <c r="E14" s="61"/>
       <c r="F14" s="60" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H14" s="81">
         <f>C25/H6</f>
@@ -5754,7 +5922,7 @@
         <v>93</v>
       </c>
       <c r="L14" s="59" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M14" s="83">
         <f>0.001*2*R9*R10*C26/R3</f>
@@ -5765,14 +5933,14 @@
       </c>
       <c r="O14" s="62"/>
       <c r="P14" s="60" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="Q14" s="61" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="R14" s="98">
         <f>2*SQRT(M20/(M2*H5))</f>
-        <v>1.4425038006176998</v>
+        <v>1.3201611530549224</v>
       </c>
       <c r="S14" s="61" t="s">
         <v>80</v>
@@ -5784,7 +5952,7 @@
         <v>189</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C15" s="59">
         <v>1.1000000000000001</v>
@@ -5797,7 +5965,7 @@
         <v>145</v>
       </c>
       <c r="G15" s="59" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H15" s="85">
         <f>H14*H13</f>
@@ -5811,7 +5979,7 @@
         <v>25</v>
       </c>
       <c r="L15" s="59" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M15" s="59">
         <f>R3*C7/120</f>
@@ -5822,10 +5990,10 @@
       </c>
       <c r="O15" s="60"/>
       <c r="P15" s="60" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="Q15" s="61" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="R15" s="61">
         <v>14</v>
@@ -5833,7 +6001,7 @@
       <c r="S15" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="T15" s="110" t="s">
+      <c r="T15" s="123" t="s">
         <v>178</v>
       </c>
     </row>
@@ -5842,7 +6010,7 @@
         <v>192</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C16" s="65">
         <f>C15*M5</f>
@@ -5856,7 +6024,7 @@
         <v>140</v>
       </c>
       <c r="G16" s="88" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H16" s="89">
         <f>H13-H15</f>
@@ -5870,7 +6038,7 @@
         <v>97</v>
       </c>
       <c r="L16" s="90" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="M16" s="90">
         <v>60</v>
@@ -5882,10 +6050,10 @@
         <v>178</v>
       </c>
       <c r="P16" s="60" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="Q16" s="61" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="R16" s="99">
         <v>1.6281399999999999</v>
@@ -5893,9 +6061,9 @@
       <c r="S16" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="T16" s="111"/>
+      <c r="T16" s="124"/>
       <c r="U16" s="70" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="V16" s="70">
         <v>0.99</v>
@@ -5903,10 +6071,10 @@
     </row>
     <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="60" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C17" s="59">
         <v>3</v>
@@ -5921,22 +6089,22 @@
         <v>137</v>
       </c>
       <c r="G17" s="59" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H17" s="59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="106" t="s">
+      <c r="J17" s="135" t="s">
         <v>178</v>
       </c>
       <c r="K17" s="58" t="s">
         <v>103</v>
       </c>
       <c r="L17" s="59" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M17" s="59">
         <f>M16*C8*C9/2</f>
@@ -5947,18 +6115,19 @@
       </c>
       <c r="O17" s="62"/>
       <c r="P17" s="60" t="s">
-        <v>337</v>
+        <v>408</v>
       </c>
       <c r="Q17" s="59" t="s">
-        <v>338</v>
-      </c>
-      <c r="R17" s="61">
-        <v>8.282</v>
+        <v>409</v>
+      </c>
+      <c r="R17" s="81">
+        <f>(R16/2)^2*M2</f>
+        <v>2.0819647548115978</v>
       </c>
       <c r="S17" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="T17" s="112"/>
+        <v>311</v>
+      </c>
+      <c r="T17" s="125"/>
       <c r="U17" s="70" t="s">
         <v>221</v>
       </c>
@@ -5971,7 +6140,7 @@
         <v>153</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C18" s="59">
         <v>0.7</v>
@@ -5986,7 +6155,7 @@
         <v>131</v>
       </c>
       <c r="G18" s="59" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H18" s="59">
         <v>1.5</v>
@@ -5994,12 +6163,12 @@
       <c r="I18" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="106"/>
+      <c r="J18" s="135"/>
       <c r="K18" s="91" t="s">
         <v>143</v>
       </c>
       <c r="L18" s="92" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="M18" s="93">
         <f>4.44*M17*M15*M14*M13/1000</f>
@@ -6010,10 +6179,10 @@
       </c>
       <c r="O18" s="94"/>
       <c r="P18" s="60" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="Q18" s="61" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="R18" s="81">
         <f>2*R10*V18+2*H13</f>
@@ -6024,7 +6193,7 @@
       </c>
       <c r="T18" s="61"/>
       <c r="U18" s="70" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="V18" s="70">
         <v>1.1000000000000001</v>
@@ -6035,7 +6204,7 @@
         <v>198</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C19" s="64">
         <f>2*M2*C18/R3</f>
@@ -6049,7 +6218,7 @@
         <v>132</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H19" s="59">
         <v>1.5</v>
@@ -6057,12 +6226,12 @@
       <c r="I19" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="106"/>
+      <c r="J19" s="135"/>
       <c r="K19" s="58" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L19" s="59" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="M19" s="64">
         <f>M18*C4*SQRT(3)*SQRT(2)</f>
@@ -6073,10 +6242,10 @@
       </c>
       <c r="O19" s="60"/>
       <c r="P19" s="60" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="Q19" s="61" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="R19" s="81">
         <f>R18*M17/1000</f>
@@ -6092,7 +6261,7 @@
         <v>198</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C20" s="64">
         <f>C19*180/M2</f>
@@ -6106,7 +6275,7 @@
         <v>146</v>
       </c>
       <c r="G20" s="59" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H20" s="59">
         <v>1.5</v>
@@ -6114,43 +6283,43 @@
       <c r="I20" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="106"/>
+      <c r="J20" s="135"/>
       <c r="K20" s="94" t="s">
         <v>67</v>
       </c>
       <c r="L20" s="92" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M20" s="95">
         <f>H5*H26/(2*M16)</f>
-        <v>6.5370800679981835</v>
+        <v>5.4752476868957016</v>
       </c>
       <c r="N20" s="96" t="s">
         <v>22</v>
       </c>
       <c r="O20" s="96"/>
       <c r="P20" s="60" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="Q20" s="61" t="s">
-        <v>362</v>
-      </c>
-      <c r="R20" s="81">
-        <f>R17*R19/1000</f>
-        <v>0.27162691034686004</v>
+        <v>357</v>
+      </c>
+      <c r="R20" s="98">
+        <f>M10*R19/R17*1000000</f>
+        <v>0.32191087501866283</v>
       </c>
       <c r="S20" s="59" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="T20" s="61"/>
       <c r="U20" s="70" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="V20" s="70" t="s">
-        <v>293</v>
-      </c>
-      <c r="W20" s="123" t="s">
-        <v>328</v>
+        <v>290</v>
+      </c>
+      <c r="W20" s="105" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6158,21 +6327,21 @@
         <v>187</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C21" s="64">
         <f>(C19*(R9/2-C13/2)+2*C13)*(R10+2*C13)/100</f>
         <v>24.520729252821194</v>
       </c>
       <c r="D21" s="59" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="60" t="s">
         <v>130</v>
       </c>
       <c r="G21" s="90" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H21" s="90">
         <v>20</v>
@@ -6189,27 +6358,27 @@
       <c r="N21" s="97"/>
       <c r="O21" s="97"/>
       <c r="P21" s="60" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="Q21" s="61" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="R21" s="81">
         <f>R20*M20^2*C6</f>
-        <v>34.82263711952983</v>
+        <v>28.951058310700411</v>
       </c>
       <c r="S21" s="61" t="s">
         <v>7</v>
       </c>
       <c r="T21" s="61"/>
       <c r="U21" s="70" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="V21" s="70" t="s">
-        <v>289</v>
-      </c>
-      <c r="W21" s="123" t="s">
-        <v>327</v>
+        <v>286</v>
+      </c>
+      <c r="W21" s="105" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6217,21 +6386,21 @@
         <v>188</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C22" s="64">
         <f>(C19*(R9/2-C13/2)+2*C13)*(R10+2*C13)/100</f>
         <v>24.520729252821194</v>
       </c>
       <c r="D22" s="59" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E22" s="61"/>
       <c r="F22" s="60" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G22" s="59" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H22" s="81">
         <f>R9+(H18+H19+H20+H21)*2</f>
@@ -6241,33 +6410,33 @@
         <v>80</v>
       </c>
       <c r="J22" s="60"/>
-      <c r="K22" s="134"/>
-      <c r="L22" s="135"/>
-      <c r="M22" s="135"/>
-      <c r="N22" s="135"/>
-      <c r="O22" s="136"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="97"/>
       <c r="P22" s="60" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="Q22" s="61" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="R22" s="81">
         <f>C4*R21</f>
-        <v>139.29054847811932</v>
+        <v>115.80423324280164</v>
       </c>
       <c r="S22" s="61" t="s">
         <v>7</v>
       </c>
       <c r="T22" s="61"/>
-      <c r="W22" s="123"/>
+      <c r="W22" s="105"/>
     </row>
     <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
         <v>203</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C23" s="64">
         <f>C22/C21</f>
@@ -6281,7 +6450,7 @@
         <v>149</v>
       </c>
       <c r="G23" s="59" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H23" s="64">
         <f>M2*H22/R2</f>
@@ -6291,22 +6460,22 @@
         <v>80</v>
       </c>
       <c r="J23" s="60"/>
-      <c r="K23" s="103" t="s">
-        <v>351</v>
-      </c>
-      <c r="L23" s="104"/>
-      <c r="M23" s="104"/>
-      <c r="N23" s="104"/>
-      <c r="O23" s="105"/>
-      <c r="P23" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q23" s="102"/>
-      <c r="R23" s="102"/>
-      <c r="S23" s="102"/>
-      <c r="T23" s="102"/>
+      <c r="K23" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="L23" s="134"/>
+      <c r="M23" s="134"/>
+      <c r="N23" s="134"/>
+      <c r="O23" s="134"/>
+      <c r="P23" s="134" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q23" s="134"/>
+      <c r="R23" s="134"/>
+      <c r="S23" s="134"/>
+      <c r="T23" s="134"/>
       <c r="W23" s="70" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6328,7 +6497,7 @@
         <v>139</v>
       </c>
       <c r="G24" s="59" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H24" s="64">
         <f>H23-H15</f>
@@ -6339,40 +6508,40 @@
       </c>
       <c r="J24" s="62"/>
       <c r="K24" s="60" t="s">
+        <v>347</v>
+      </c>
+      <c r="L24" s="61" t="s">
         <v>352</v>
       </c>
-      <c r="L24" s="61" t="s">
-        <v>357</v>
-      </c>
-      <c r="M24" s="81">
-        <f>C17*R10*C18*M2*(R9-C13)/R3/1000</f>
-        <v>6.6103768836310586</v>
+      <c r="M24" s="116">
+        <f>C17*R10*C18*M2*(R9-C13)/1000</f>
+        <v>132.20753767262116</v>
       </c>
       <c r="N24" s="61" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="124" t="s">
+      <c r="P24" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="Q24" s="125" t="s">
-        <v>349</v>
-      </c>
-      <c r="R24" s="126">
-        <f>C26</f>
-        <v>0.99297177075985155</v>
-      </c>
-      <c r="S24" s="125" t="s">
+      <c r="Q24" s="107" t="s">
+        <v>344</v>
+      </c>
+      <c r="R24" s="108">
+        <f>C25*2/M2</f>
+        <v>0.57490900209566576</v>
+      </c>
+      <c r="S24" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="T24" s="125"/>
+      <c r="T24" s="107"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C25" s="98">
         <f>V16*C14*C23/(1+V17*C15*C24)</f>
@@ -6381,54 +6550,54 @@
       <c r="D25" s="61"/>
       <c r="E25" s="61"/>
       <c r="F25" s="60" t="s">
-        <v>150</v>
+        <v>410</v>
       </c>
       <c r="G25" s="59" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H25" s="64">
-        <f>(H24+H15)*H21/2</f>
-        <v>326.85400339990917</v>
+        <f>(H24+H16-3)*(H21-1.5)/2</f>
+        <v>273.76238434478512</v>
       </c>
       <c r="I25" s="59" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J25" s="59"/>
       <c r="K25" s="70" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="L25" s="61" t="s">
-        <v>389</v>
-      </c>
-      <c r="M25" s="139">
-        <f>0</f>
-        <v>0</v>
+        <v>383</v>
+      </c>
+      <c r="M25" s="126">
+        <f>(M2/4*(H29^2-R9^2)-R2*H21*(H16+H24)/2)*R10/1000</f>
+        <v>1576.2377096665907</v>
       </c>
       <c r="N25" s="61" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="O25" s="61"/>
-      <c r="P25" s="127" t="s">
+      <c r="P25" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="Q25" s="128" t="s">
+      <c r="Q25" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="R25" s="129">
+      <c r="R25" s="111">
         <f>R2*M16*C9*M20/(M2*R9)</f>
-        <v>29.859548249533173</v>
-      </c>
-      <c r="S25" s="128" t="s">
+        <v>25.009395752295156</v>
+      </c>
+      <c r="S25" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="T25" s="128"/>
+      <c r="T25" s="110"/>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C26" s="98">
         <f>C25*C18*M2/2</f>
@@ -6437,200 +6606,205 @@
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
       <c r="F26" s="60" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G26" s="59" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H26" s="81">
         <f>H25*H2</f>
-        <v>196.11240203994549</v>
+        <v>164.25743060687105</v>
       </c>
       <c r="I26" s="59" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J26" s="60"/>
       <c r="K26" s="60" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="L26" s="61" t="s">
-        <v>391</v>
-      </c>
-      <c r="M26" s="137">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="61" t="s">
-        <v>356</v>
+        <v>385</v>
+      </c>
+      <c r="M26" s="145">
+        <f>(M2/4*((R9-2*C17-2*C13)^2-R11^2)*R10/1000)</f>
+        <v>2483.2339162640374</v>
+      </c>
+      <c r="N26" s="59" t="s">
+        <v>351</v>
       </c>
       <c r="O26" s="61"/>
-      <c r="P26" s="124" t="s">
+      <c r="P26" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="Q26" s="125" t="s">
+      <c r="Q26" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="R26" s="130">
+      <c r="R26" s="112">
         <f>M16*C9*M20/(M2*(R16/2)*M16)</f>
-        <v>5.1121333909774558</v>
-      </c>
-      <c r="S26" s="125" t="s">
+        <v>4.2817582518341242</v>
+      </c>
+      <c r="S26" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="T26" s="125"/>
+      <c r="T26" s="107"/>
     </row>
     <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="119" t="s">
-        <v>345</v>
-      </c>
-      <c r="B27" s="120" t="s">
-        <v>347</v>
-      </c>
-      <c r="C27" s="121">
+      <c r="A27" s="101" t="s">
+        <v>340</v>
+      </c>
+      <c r="B27" s="102" t="s">
+        <v>342</v>
+      </c>
+      <c r="C27" s="103">
         <f>4*C25/M2*(COS(M2*C18/2))</f>
         <v>0.52200645161955517</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
-      <c r="F27" s="103" t="s">
-        <v>318</v>
-      </c>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="104"/>
-      <c r="J27" s="105"/>
+      <c r="F27" s="130" t="s">
+        <v>315</v>
+      </c>
+      <c r="G27" s="131"/>
+      <c r="H27" s="131"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="132"/>
       <c r="K27" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="L27" s="61" t="s">
         <v>353</v>
       </c>
-      <c r="L27" s="61" t="s">
-        <v>358</v>
-      </c>
-      <c r="M27" s="81">
+      <c r="M27" s="145">
         <f>R19*C6*C4*(R16/2)^2*M2</f>
         <v>819.39288162356786</v>
       </c>
-      <c r="N27" s="61" t="s">
-        <v>356</v>
+      <c r="N27" s="59" t="s">
+        <v>351</v>
       </c>
       <c r="O27" s="61"/>
-      <c r="P27" s="131" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q27" s="132" t="s">
-        <v>378</v>
-      </c>
-      <c r="R27" s="133">
+      <c r="P27" s="113" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q27" s="114" t="s">
+        <v>372</v>
+      </c>
+      <c r="R27" s="115">
         <f>C2/M29</f>
-        <v>94.705819430916407</v>
-      </c>
-      <c r="S27" s="132" t="s">
-        <v>379</v>
-      </c>
-      <c r="T27" s="132"/>
+        <v>95.749247573146022</v>
+      </c>
+      <c r="S27" s="114" t="s">
+        <v>373</v>
+      </c>
+      <c r="T27" s="114"/>
+      <c r="V27" s="70">
+        <f>R17*M16*C9</f>
+        <v>249.83577057739174</v>
+      </c>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
-        <v>346</v>
-      </c>
-      <c r="B28" s="120" t="s">
-        <v>348</v>
-      </c>
-      <c r="C28" s="122">
+      <c r="A28" s="101" t="s">
+        <v>341</v>
+      </c>
+      <c r="B28" s="102" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="104">
         <f>C27*2/M2</f>
         <v>0.33231962878418064</v>
       </c>
       <c r="D28" s="61"/>
       <c r="E28" s="61"/>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="120" t="s">
         <v>135</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>136</v>
       </c>
       <c r="H28" s="23">
-        <f>(H6/H7)*H15/2</f>
-        <v>9.1248861612296661</v>
+        <f>C25*C18*R9*M2/(H7*2*R3)</f>
+        <v>7.6649043754329176</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>80</v>
       </c>
       <c r="J28" s="60"/>
       <c r="K28" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="L28" s="61" t="s">
         <v>354</v>
       </c>
-      <c r="L28" s="61" t="s">
-        <v>359</v>
-      </c>
-      <c r="M28" s="81">
+      <c r="M28" s="145">
         <f>M2*R9*R10/1000</f>
         <v>63.271226104450712</v>
       </c>
-      <c r="N28" s="61" t="s">
-        <v>356</v>
+      <c r="N28" s="59" t="s">
+        <v>351</v>
       </c>
       <c r="O28" s="61"/>
-      <c r="P28" s="131" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q28" s="132" t="s">
-        <v>381</v>
-      </c>
-      <c r="R28" s="133">
+      <c r="P28" s="113" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q28" s="114" t="s">
+        <v>375</v>
+      </c>
+      <c r="R28" s="115">
         <f>M20*M18</f>
-        <v>649.86469631032458</v>
-      </c>
-      <c r="S28" s="132" t="s">
+        <v>544.30573562760139</v>
+      </c>
+      <c r="S28" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="T28" s="132"/>
+      <c r="T28" s="114"/>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="60" t="s">
-        <v>324</v>
+      <c r="A29" s="60"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="120" t="s">
+        <v>321</v>
       </c>
       <c r="G29" s="61" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H29" s="73">
         <f>H22+H28*2</f>
-        <v>267.94783809804039</v>
+        <v>265.02787452644691</v>
       </c>
       <c r="I29" s="61" t="s">
         <v>80</v>
       </c>
       <c r="J29" s="60"/>
       <c r="K29" s="60" t="s">
+        <v>350</v>
+      </c>
+      <c r="L29" s="61" t="s">
         <v>355</v>
       </c>
-      <c r="L29" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="M29" s="137">
+      <c r="M29" s="145">
         <f>M2*H29*R10/1000</f>
-        <v>84.472105812205513</v>
-      </c>
-      <c r="N29" s="61" t="s">
-        <v>356</v>
+        <v>83.551570406739074</v>
+      </c>
+      <c r="N29" s="59" t="s">
+        <v>351</v>
       </c>
       <c r="O29" s="60"/>
-      <c r="P29" s="131" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q29" s="132" t="s">
+      <c r="P29" s="113" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q29" s="114" t="s">
         <v>239</v>
       </c>
-      <c r="R29" s="133">
+      <c r="R29" s="115">
         <f>R28*C4*C6</f>
-        <v>7798.3763557238944</v>
-      </c>
-      <c r="S29" s="132" t="s">
+        <v>6531.6688275312172</v>
+      </c>
+      <c r="S29" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="T29" s="132"/>
+      <c r="T29" s="114"/>
     </row>
     <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
@@ -6638,35 +6812,49 @@
       <c r="C30" s="98"/>
       <c r="D30" s="61"/>
       <c r="E30" s="61"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
+      <c r="F30" s="120" t="s">
+        <v>398</v>
+      </c>
+      <c r="G30" s="61" t="s">
+        <v>399</v>
+      </c>
+      <c r="H30" s="73">
+        <f>H22</f>
+        <v>249.69806577558106</v>
+      </c>
+      <c r="I30" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="60"/>
       <c r="K30" s="60" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="L30" s="61" t="s">
-        <v>373</v>
-      </c>
-      <c r="M30" s="138">
-        <f>M24*M8</f>
-        <v>48.916788938869836</v>
-      </c>
-      <c r="N30" s="61" t="s">
-        <v>376</v>
+        <v>368</v>
+      </c>
+      <c r="M30" s="146">
+        <f>M24*M8/1000</f>
+        <v>0.97833577877739664</v>
+      </c>
+      <c r="N30" s="59" t="s">
+        <v>371</v>
       </c>
       <c r="O30" s="60"/>
-      <c r="P30" s="131" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q30" s="132" t="s">
-        <v>395</v>
-      </c>
-      <c r="R30" s="132"/>
-      <c r="S30" s="132" t="s">
+      <c r="P30" s="113" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q30" s="114" t="s">
+        <v>389</v>
+      </c>
+      <c r="R30" s="114">
+        <v>1.08</v>
+      </c>
+      <c r="S30" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="T30" s="132"/>
+      <c r="T30" s="127" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
@@ -6679,31 +6867,33 @@
       <c r="H31" s="61"/>
       <c r="I31" s="61"/>
       <c r="J31" s="61"/>
-      <c r="K31" s="60" t="s">
+      <c r="K31" s="70" t="s">
+        <v>411</v>
+      </c>
+      <c r="L31" s="61" t="s">
+        <v>412</v>
+      </c>
+      <c r="M31" s="146">
+        <f>M7*M25/1000</f>
+        <v>12.058218478949421</v>
+      </c>
+      <c r="N31" s="59" t="s">
         <v>371</v>
       </c>
-      <c r="L31" s="61" t="s">
-        <v>374</v>
-      </c>
-      <c r="M31" s="138">
-        <f>M26*M7/1000</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="61" t="s">
-        <v>377</v>
-      </c>
       <c r="O31" s="60"/>
-      <c r="P31" s="131" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q31" s="132" t="s">
-        <v>397</v>
-      </c>
-      <c r="R31" s="132"/>
-      <c r="S31" s="132" t="s">
+      <c r="P31" s="113" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q31" s="114" t="s">
+        <v>391</v>
+      </c>
+      <c r="R31" s="114">
+        <v>1.69</v>
+      </c>
+      <c r="S31" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="T31" s="132"/>
+      <c r="T31" s="128"/>
     </row>
     <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
@@ -6716,30 +6906,32 @@
       <c r="H32" s="61"/>
       <c r="I32" s="61"/>
       <c r="J32" s="61"/>
-      <c r="K32" s="140" t="s">
-        <v>372</v>
-      </c>
-      <c r="L32" s="141" t="s">
-        <v>375</v>
-      </c>
-      <c r="M32" s="142">
-        <f>M27*M6/1000</f>
-        <v>7.3417602193471687</v>
-      </c>
-      <c r="N32" s="141" t="s">
-        <v>377</v>
-      </c>
-      <c r="P32" s="131" t="s">
-        <v>398</v>
-      </c>
-      <c r="Q32" s="132" t="s">
-        <v>399</v>
-      </c>
-      <c r="R32" s="132"/>
-      <c r="S32" s="132" t="s">
+      <c r="K32" s="60" t="s">
+        <v>366</v>
+      </c>
+      <c r="L32" s="61" t="s">
+        <v>369</v>
+      </c>
+      <c r="M32" s="146">
+        <f>M26*M7/1000</f>
+        <v>18.996739459419885</v>
+      </c>
+      <c r="N32" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="P32" s="113" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q32" s="114" t="s">
+        <v>393</v>
+      </c>
+      <c r="R32" s="114">
+        <v>0.18</v>
+      </c>
+      <c r="S32" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="T32" s="125"/>
+      <c r="T32" s="128"/>
     </row>
     <row r="33" spans="1:20" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
@@ -6752,30 +6944,50 @@
       <c r="H33" s="61"/>
       <c r="I33" s="61"/>
       <c r="J33" s="61"/>
-      <c r="K33" s="60" t="s">
-        <v>392</v>
-      </c>
-      <c r="L33" s="60" t="s">
-        <v>393</v>
-      </c>
-      <c r="M33" s="61"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="143"/>
-      <c r="P33" s="124" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q33" s="125" t="s">
-        <v>401</v>
-      </c>
-      <c r="R33" s="125"/>
-      <c r="S33" s="125" t="s">
+      <c r="K33" s="117" t="s">
+        <v>367</v>
+      </c>
+      <c r="L33" s="118" t="s">
+        <v>370</v>
+      </c>
+      <c r="M33" s="146">
+        <f>M27*M6/1000</f>
+        <v>7.3417602193471687</v>
+      </c>
+      <c r="N33" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="O33" s="119"/>
+      <c r="P33" s="106" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q33" s="107" t="s">
+        <v>395</v>
+      </c>
+      <c r="R33" s="107">
+        <v>3.97</v>
+      </c>
+      <c r="S33" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="T33" s="125"/>
-    </row>
-    <row r="34" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="T33" s="128"/>
+    </row>
+    <row r="34" spans="1:20" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="K34" s="60" t="s">
+        <v>386</v>
+      </c>
+      <c r="L34" s="60" t="s">
+        <v>387</v>
+      </c>
+      <c r="M34" s="64">
+        <f>SUM(M30:M33)</f>
+        <v>39.37505393649387</v>
+      </c>
+      <c r="N34" s="59" t="s">
+        <v>371</v>
+      </c>
       <c r="P34" s="60" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="Q34" s="59" t="s">
         <v>240</v>
@@ -6784,38 +6996,24 @@
       <c r="S34" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="T34" s="60"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P44" s="60"/>
-      <c r="Q44" s="61"/>
-      <c r="R44" s="81"/>
-      <c r="S44" s="61"/>
-      <c r="T44" s="60"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P45" s="60"/>
-      <c r="Q45" s="61"/>
-      <c r="R45" s="81"/>
-      <c r="S45" s="61"/>
-      <c r="T45" s="60"/>
+      <c r="T34" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="J17:J20"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="T30:T34"/>
     <mergeCell ref="F27:J27"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="A12:E12"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="J17:J20"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="F12:J12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="W20" r:id="rId1"/>
@@ -6903,10 +7101,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="77" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7811,12 +8009,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="113" t="s">
+      <c r="F7" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -8077,35 +8275,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="143" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117" t="s">
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="114" t="s">
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
+      <c r="O1" s="143"/>
+      <c r="P1" s="140" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="116"/>
+      <c r="Q1" s="141"/>
+      <c r="R1" s="141"/>
+      <c r="S1" s="141"/>
+      <c r="T1" s="141"/>
+      <c r="U1" s="142"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8327,7 +8525,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="144" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -8394,7 +8592,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="118"/>
+      <c r="J6" s="144"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -8621,20 +8819,20 @@
       <c r="E10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="143" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117" t="s">
+      <c r="G10" s="143"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="143"/>
+      <c r="J10" s="143"/>
+      <c r="K10" s="143" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
+      <c r="L10" s="143"/>
+      <c r="M10" s="143"/>
+      <c r="N10" s="143"/>
+      <c r="O10" s="143"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -8699,7 +8897,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="118" t="s">
+      <c r="O11" s="144" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -8766,7 +8964,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="118"/>
+      <c r="O12" s="144"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -8832,7 +9030,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="118"/>
+      <c r="O13" s="144"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -8997,13 +9195,13 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="117" t="s">
+      <c r="F17" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="117"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="117"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="143"/>
+      <c r="I17" s="143"/>
+      <c r="J17" s="143"/>
       <c r="K17" s="29" t="s">
         <v>140</v>
       </c>
@@ -9242,13 +9440,13 @@
         <v>15</v>
       </c>
       <c r="J23" s="46"/>
-      <c r="K23" s="117" t="s">
+      <c r="K23" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="117"/>
-      <c r="M23" s="117"/>
-      <c r="N23" s="117"/>
-      <c r="O23" s="117"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="44"/>

</xml_diff>